<commit_message>
#4 ajout des cartes/faces
un tableau avec toutes les exploits(cartes)
et un autre avec toutes les faces pour le dés avec pour chaque tableau leur valeur leur effet leur récompense etc..
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\PS5-18-19-DiceForge-EquipeG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AE358039-5FDA-4A90-AE4F-A83E78A0ACCB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B52BADC7-46CB-42D1-A988-BDD2D36E1ABB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{CDF5D2E8-3819-49DE-A1AD-AC0A83541AB5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="95">
   <si>
     <t>Numéro</t>
   </si>
@@ -96,43 +96,243 @@
     <t>http://jeuxstrategie1.free.fr/jeu_dice_forge/guide.pdf</t>
   </si>
   <si>
-    <t>cartes dés : 1/3/4/6G</t>
-  </si>
-  <si>
-    <t>1/2 pierre de feu</t>
-  </si>
-  <si>
-    <t>1/2 pierre de lune</t>
-  </si>
-  <si>
-    <t>2/3/4 honneur</t>
-  </si>
-  <si>
-    <t>2G/1pierre de lune</t>
-  </si>
-  <si>
-    <t>1honor/1pierre de feu</t>
-  </si>
-  <si>
-    <t>1ALL</t>
-  </si>
-  <si>
-    <t>2honor/2lunes</t>
-  </si>
-  <si>
-    <t>3G OU 2honor</t>
-  </si>
-  <si>
-    <t>x3 everything x3x3 doesn't work</t>
-  </si>
-  <si>
-    <t>copie face ennemie fonctionne avec le x3</t>
+    <t>chest</t>
+  </si>
+  <si>
+    <t>marteau</t>
+  </si>
+  <si>
+    <t>PRIX</t>
+  </si>
+  <si>
+    <t>CARTE</t>
+  </si>
+  <si>
+    <t>ACTION</t>
+  </si>
+  <si>
+    <t>REPETITIVITE ?</t>
+  </si>
+  <si>
+    <t>RECOMPENSE</t>
+  </si>
+  <si>
+    <t>1PdL</t>
+  </si>
+  <si>
+    <t>Les sabots d'argent</t>
+  </si>
+  <si>
+    <t>2PdL</t>
+  </si>
+  <si>
+    <t>oui</t>
+  </si>
+  <si>
+    <t>2honor</t>
+  </si>
+  <si>
+    <t>Les satyres</t>
+  </si>
+  <si>
+    <t>3PdL</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>6honor</t>
+  </si>
+  <si>
+    <t>Le passeur</t>
+  </si>
+  <si>
+    <t>4PdL</t>
+  </si>
+  <si>
+    <t>aucune</t>
+  </si>
+  <si>
+    <t>12honor</t>
+  </si>
+  <si>
+    <t>Le casque d'invisibilité</t>
+  </si>
+  <si>
+    <t>5PdL</t>
+  </si>
+  <si>
+    <t>x3 une face du dé</t>
+  </si>
+  <si>
+    <t>4honor</t>
+  </si>
+  <si>
+    <t>8honor</t>
+  </si>
+  <si>
+    <t>6PdL</t>
+  </si>
+  <si>
+    <t>relance deux fois les dés</t>
+  </si>
+  <si>
+    <t>La pince</t>
+  </si>
+  <si>
+    <t>L'Hydre</t>
+  </si>
+  <si>
+    <t>26honor</t>
+  </si>
+  <si>
+    <t>L'ancien</t>
+  </si>
+  <si>
+    <t>1PdF</t>
+  </si>
+  <si>
+    <t>5PdL+5PdF</t>
+  </si>
+  <si>
+    <t>0honor</t>
+  </si>
+  <si>
+    <t>3G=4honor</t>
+  </si>
+  <si>
+    <t>Les herbes folles</t>
+  </si>
+  <si>
+    <t>3G+3PdL</t>
+  </si>
+  <si>
+    <t>Les ailes de la gardienne</t>
+  </si>
+  <si>
+    <t>2PdF</t>
+  </si>
+  <si>
+    <t>1G ou 1PdF ou 1PdL</t>
+  </si>
+  <si>
+    <t>Le minotaure</t>
+  </si>
+  <si>
+    <t>3PdF</t>
+  </si>
+  <si>
+    <t>tlm lance les dés et retire 
+le résultats à ses reserves</t>
+  </si>
+  <si>
+    <t>La méduse</t>
+  </si>
+  <si>
+    <t>4PdF</t>
+  </si>
+  <si>
+    <t>14honor</t>
+  </si>
+  <si>
+    <t>Le mirroir abyssal</t>
+  </si>
+  <si>
+    <t>5PdF</t>
+  </si>
+  <si>
+    <t>forge une face sur son dé
+ permettant de copier le 
+résultat du dé d'un adversaire</t>
+  </si>
+  <si>
+    <t>10honor</t>
+  </si>
+  <si>
+    <t>L'énigme</t>
+  </si>
+  <si>
+    <t>6PdF</t>
+  </si>
+  <si>
+    <t>relance 4 fois UN dé</t>
+  </si>
+  <si>
+    <t>FACES</t>
+  </si>
+  <si>
+    <t>2G</t>
+  </si>
+  <si>
+    <t>4G</t>
+  </si>
+  <si>
+    <t>6G</t>
+  </si>
+  <si>
+    <t>3G</t>
+  </si>
+  <si>
+    <t>8G</t>
+  </si>
+  <si>
+    <t>3honor</t>
+  </si>
+  <si>
+    <t>12G</t>
+  </si>
+  <si>
+    <t>2G+1PdL</t>
+  </si>
+  <si>
+    <t>1honor+1PdF</t>
+  </si>
+  <si>
+    <t>3G+2honor</t>
+  </si>
+  <si>
+    <t>5G</t>
+  </si>
+  <si>
+    <t>1G+1PdF+1PdL+1honor</t>
+  </si>
+  <si>
+    <t>2PdF ou 2PdL ou 2G</t>
+  </si>
+  <si>
+    <t>2honor+2PdL</t>
+  </si>
+  <si>
+    <t>relance UN dé</t>
+  </si>
+  <si>
+    <t>tlm lance les dés et vous 
+choisissez deux faces chez 
+les dés des ennemis que 
+vous prennez, les autres ne
+ reçoivent rien</t>
+  </si>
+  <si>
+    <t>à chaque fois que vous avez
+ de l'or vous choisissez si 
+vous le gardez ou le mettez
+ dans le marteau à 15G vous
+ avez 10honor puis vous 
+pouvez recommencer pour 
+15honor et le marteau est 
+détruit</t>
+  </si>
+  <si>
+    <t>augmente vos réserves 
+maximales de +4G +3PdL 
++3PdF pour chaque chest 
+acquis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -163,7 +363,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,8 +388,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -268,11 +480,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -301,12 +528,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Style de tableau 1" pivot="0" count="0" xr9:uid="{71D47326-84C0-4818-B420-08AD473B989B}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -615,16 +850,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07200E0C-4973-414C-A209-F8996EA50DD1}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.140625" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -760,7 +999,7 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <f t="shared" ref="A7:A12" si="0">A6+1</f>
         <v>6</v>
@@ -779,7 +1018,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
     </row>
-    <row r="8" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -866,54 +1105,393 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C17" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" ht="166.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="D19" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+      <c r="F19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
+      <c r="I20" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="108" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H32" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Small file changes"
This reverts commit 155dba1c6250b4758bc8d8e1e285ff72a2619eed.
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bibi/Documents/PS5-18-19-DiceForge-EquipeG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\PS5-18-19-DiceForge-EquipeG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBB9C01-5EF0-E148-8850-9EFADC95A596}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9E4A4601-A912-43D9-9FF9-1B9BA37404F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16180" xr2:uid="{CDF5D2E8-3819-49DE-A1AD-AC0A83541AB5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{CDF5D2E8-3819-49DE-A1AD-AC0A83541AB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,6 +69,9 @@
     <t>créer une AI basique</t>
   </si>
   <si>
+    <t>http://jeuxstrategie1.free.fr/jeu_dice_forge/guide.pdf</t>
+  </si>
+  <si>
     <t>chest</t>
   </si>
   <si>
@@ -99,6 +102,9 @@
     <t>oui</t>
   </si>
   <si>
+    <t>2honor</t>
+  </si>
+  <si>
     <t>Les satyres</t>
   </si>
   <si>
@@ -108,6 +114,9 @@
     <t>non</t>
   </si>
   <si>
+    <t>6honor</t>
+  </si>
+  <si>
     <t>Le passeur</t>
   </si>
   <si>
@@ -117,6 +126,9 @@
     <t>aucune</t>
   </si>
   <si>
+    <t>12honor</t>
+  </si>
+  <si>
     <t>Le casque d'invisibilité</t>
   </si>
   <si>
@@ -126,6 +138,12 @@
     <t>x3 une face du dé</t>
   </si>
   <si>
+    <t>4honor</t>
+  </si>
+  <si>
+    <t>8honor</t>
+  </si>
+  <si>
     <t>6PdL</t>
   </si>
   <si>
@@ -138,9 +156,24 @@
     <t>L'Hydre</t>
   </si>
   <si>
+    <t>26honor</t>
+  </si>
+  <si>
     <t>L'ancien</t>
   </si>
   <si>
+    <t>1PdF</t>
+  </si>
+  <si>
+    <t>5PdL+5PdF</t>
+  </si>
+  <si>
+    <t>0honor</t>
+  </si>
+  <si>
+    <t>3G=4honor</t>
+  </si>
+  <si>
     <t>Les herbes folles</t>
   </si>
   <si>
@@ -150,7 +183,16 @@
     <t>Les ailes de la gardienne</t>
   </si>
   <si>
+    <t>2PdF</t>
+  </si>
+  <si>
+    <t>1G ou 1PdF ou 1PdL</t>
+  </si>
+  <si>
     <t>Le minotaure</t>
+  </si>
+  <si>
+    <t>3PdF</t>
   </si>
   <si>
     <t>tlm lance les dés et retire 
@@ -158,6 +200,15 @@
   </si>
   <si>
     <t>La méduse</t>
+  </si>
+  <si>
+    <t>4PdF</t>
+  </si>
+  <si>
+    <t>14honor</t>
+  </si>
+  <si>
+    <t>5PdF</t>
   </si>
   <si>
     <t>forge une face sur son dé
@@ -165,9 +216,15 @@
 résultat du dé d'un adversaire</t>
   </si>
   <si>
+    <t>10honor</t>
+  </si>
+  <si>
     <t>L'énigme</t>
   </si>
   <si>
+    <t>6PdF</t>
+  </si>
+  <si>
     <t>relance 4 fois UN dé</t>
   </si>
   <si>
@@ -189,13 +246,28 @@
     <t>8G</t>
   </si>
   <si>
+    <t>3honor</t>
+  </si>
+  <si>
     <t>12G</t>
   </si>
   <si>
     <t>2G+1PdL</t>
   </si>
   <si>
+    <t>1honor+1PdF</t>
+  </si>
+  <si>
     <t>5G</t>
+  </si>
+  <si>
+    <t>1G+1PdF+1PdL+1honor</t>
+  </si>
+  <si>
+    <t>2PdF ou 2PdL ou 2G</t>
+  </si>
+  <si>
+    <t>2honor+2PdL</t>
   </si>
   <si>
     <t>relance UN dé</t>
@@ -208,536 +280,464 @@
  reçoivent rien</t>
   </si>
   <si>
-    <t>Stéphane</t>
-  </si>
-  <si>
-    <t>création de dé</t>
-  </si>
-  <si>
-    <t>création d'une face 1G</t>
-  </si>
-  <si>
-    <t>création d'une face permettant d'obtenir 1gold, cette dernière devra être mise sur un dé pour être utilisée</t>
-  </si>
-  <si>
-    <t>DÉ 1</t>
-  </si>
-  <si>
-    <t>DÉ 2</t>
-  </si>
-  <si>
-    <t>BASSIN</t>
-  </si>
-  <si>
-    <t>1 à 2G</t>
-  </si>
-  <si>
-    <t>2 à 3G</t>
-  </si>
-  <si>
-    <t>3 à 4G</t>
-  </si>
-  <si>
-    <t>4 à 5G</t>
-  </si>
-  <si>
-    <t>5 à 6G</t>
-  </si>
-  <si>
-    <t>6 à 8G</t>
-  </si>
-  <si>
-    <t>7 à 12G</t>
-  </si>
-  <si>
-    <t>création d'une classe dice qui sera utilisable par chaque joueur et qui retournera un résultat entre 1 et 6 qui, plus tard, sera le numéro de la face qu'il aura obtenu (objet qui contiendra les objets faces)</t>
-  </si>
-  <si>
-    <t>création d'une face PdL</t>
-  </si>
-  <si>
-    <t>Il s'agit d'un exploit(carte dans le tableau ci-dessous) récompensant le joueur contre certaines ressources, durant cette slice on ne créera qu'un seul exploit demandant UNE PdL</t>
-  </si>
-  <si>
-    <t>création d'exploit(carte), marteau</t>
-  </si>
-  <si>
-    <t>création de l'exploit, chest</t>
-  </si>
-  <si>
-    <t>Création de l'exploit qui est décrit dans le tableau si dessous nommé chest, il sera sur la même ile que "marteau"</t>
-  </si>
-  <si>
-    <t>Ile</t>
-  </si>
-  <si>
-    <t>1,lune</t>
-  </si>
-  <si>
-    <t>1lune</t>
-  </si>
-  <si>
-    <t>2,lune</t>
-  </si>
-  <si>
-    <t>3,lune</t>
-  </si>
-  <si>
-    <t>4,lune+soleil</t>
-  </si>
-  <si>
-    <t>1,soleil</t>
-  </si>
-  <si>
-    <t>2,soleil</t>
-  </si>
-  <si>
-    <t>3,soleil</t>
-  </si>
-  <si>
-    <t>création de l'ile 1,soleil</t>
-  </si>
-  <si>
-    <t>création de l'ile 1,lune</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'ile se trouvant en dessous de celle 1,lune et possédant deux exploit,"L'ancien" et "Les herbes folles"</t>
-  </si>
-  <si>
-    <t>Il s'agit d'un élément contenant plusieurs exploits, de plus deux joueurs ne peuvent pas être tout les deux sur une même ile, celui qui est arrivé en premier est renvoyé au spawn et peut relancer ses dés (faveur des dieux), durant cette slice on ne créera qu'une seule ile. la première ile créée sera l'ile 1,lune. cette ile possède deux exploit "marteau" et "chest"</t>
-  </si>
-  <si>
-    <t>création de l'exploit "L'ancien"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "L'ancien" décrit dans le tableau ci-dessous</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Les herbes folles"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "Les herbes folles" décrit dans le tableau ci-dessous</t>
-  </si>
-  <si>
-    <t>amelioration de l'AI pour qu'il y en ait une qui cherche à avoir le plus d'honneur via l'argent, strat marteau + ancien</t>
-  </si>
-  <si>
-    <t>l'AI developpée va chercher à réaliser la stratégie reposant sur l'argent où elle cherche à avoir le plus d'or obtenu sur ses dés, puis elle achete des anciens et enfin des marteaux, dès qu'elle a suffisament d'or à donner à ses anciens pour le tour suivant, elle donne tout son or aux marteaux.</t>
-  </si>
-  <si>
-    <t>création du bassin à 2G</t>
-  </si>
-  <si>
-    <t>il s'agit d'un objet possédant un nombre de case égal au nombre de joueur et possédant pour chaque bassin des faces spécifiques, le bassin a un prix pour acheter une face et on ne peut pas acheter durant le même tour deux faces du même bassin ce bassin possédera uniquement des objets coutant 2G, ici le seul objet créer à 2G est la face donnant 3G</t>
-  </si>
-  <si>
-    <t>création d'une face 3G</t>
-  </si>
-  <si>
-    <t>cette face ira dans le bassin à 2G</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face étant dans un bassin à 2G et qui, quand elle est obtenue en lancant le dé donne une PdL, elle se trouve dans le bassin à 2G</t>
-  </si>
-  <si>
-    <t>création du bassin à 3G</t>
-  </si>
-  <si>
-    <t>3G/1PdL</t>
-  </si>
-  <si>
-    <t>création de l'ile 2,lune</t>
-  </si>
-  <si>
-    <t>création de l'ile 3,lune</t>
-  </si>
-  <si>
-    <t>CARTE/EXPLOIT</t>
-  </si>
-  <si>
-    <t>il s'agit de la deuxième ile de la partie lune du plateau elle comporte deux exploits "Les sabots d'argent" et "Les satyres"</t>
-  </si>
-  <si>
-    <t>il s'agit de l'exploit "Les sabots d'argent" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,lune</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Les sabots d'argent"</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Les satyres"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "Les satyres" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,lune</t>
-  </si>
-  <si>
-    <t>il s'agit de la troisième ile de la partie lune du plateau elle comporte deux exploits "Le passeur" et "Le casque d'invisibilité"</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Le passeur"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "Le passeur" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,lune</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Le casque d'invisibilité"</t>
-  </si>
-  <si>
-    <t>il s'agit de l'exploit "Le casque d'invisibilité" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,lune</t>
-  </si>
-  <si>
-    <t>création du bassin à 12G</t>
-  </si>
-  <si>
-    <t>il s'agit du bassin à 12G décrit dans le tableau ci-dessous</t>
-  </si>
-  <si>
-    <t>création du bassin à 5G</t>
-  </si>
-  <si>
-    <t>Il s'agit du bassin à 5G décrit dans le tableau ci-dessous</t>
-  </si>
-  <si>
-    <t>création du bassin à 8G</t>
-  </si>
-  <si>
-    <t>il s'agit du bassin à 8G décrit dans le tableau ci-dessous</t>
-  </si>
-  <si>
-    <t>création de la face 2PdL</t>
-  </si>
-  <si>
-    <t>Il s'agit de la face 2PdL se trouvant dans le bassin à 6G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">création du bassin 6G </t>
-  </si>
-  <si>
-    <t>il s'agit du bassin 6G décrit dans le tableau ci-dessous</t>
-  </si>
-  <si>
-    <t>création d'une AI PdL</t>
-  </si>
-  <si>
-    <t>Il s'agit d'une AI qui cherchera à obtenir sur son dé un maximum de face lui donnant des PdL puis sur les iles elle achetera l'objet coutant le plus de PdL dès qu'elle le peut</t>
-  </si>
-  <si>
-    <t>création de l'ile 2,soleil</t>
-  </si>
-  <si>
-    <t>Il s'agit de la deuxième ile de la partie soleil du plateau elle comporte deux exploits "Les ailes de la gardienne" et "Le minotaure"</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Les ailes de la gardienne"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "Les ailes de la gardienne" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,soleil</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Le minotaure"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "Le minotaure" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,soleil</t>
-  </si>
-  <si>
-    <t>création de l'ile 3,soleil</t>
-  </si>
-  <si>
-    <t>Il s'agit de la troisième ile de la partie soleil du plateau elle comporte deux exploits "La méduse" et "Le miroir abyssal"</t>
-  </si>
-  <si>
-    <t>Le miroir abyssal</t>
-  </si>
-  <si>
-    <t>création de l'exploit "La méduse"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "La méduse" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,soleil</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Le miroir abyssal"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "Le miroir abyssal" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,soleil</t>
-  </si>
-  <si>
-    <t>création d'une face 2G +1PdL</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face produisant 2G + 1PdL quand on tombe sur elle, elle se situe dans le bassin à 4G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face produisant un de toute les ressources, elle se situe dans le bassin à 12G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t>création de l'ile 4,lune+soleil</t>
-  </si>
-  <si>
-    <t>Il s'agit de la quatrième ile des deux parcours lune et soleil, elle comporte trois exploits "La pince", "L'Hydre" et "L'énigme"</t>
-  </si>
-  <si>
-    <t>création de l'exploit "La pince"</t>
-  </si>
-  <si>
-    <t>création de l'exploit "L'Hydre"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "La pince" qui est décrit dans le tableau ci-dessous, il se trouve sur l'ile 4,lune+soleil, partie lune</t>
-  </si>
-  <si>
-    <t>il s'agit de l'exploit "L'Hydre" qui est décrit dans le tableau ci-dessous, il se trouve sur l'ile 4,lune+soleil,partie centrale</t>
-  </si>
-  <si>
-    <t>création de l'exploit "L'énigme"</t>
-  </si>
-  <si>
-    <t>il s'agit de l'exploit "L'énigme" qui est décrit dans letableau ci-dessous, il se trouve sur l'ile 4,lune+soleil, partie soleil</t>
-  </si>
-  <si>
-    <t>création d'une AI multi-ressources</t>
-  </si>
-  <si>
-    <t>5x1G</t>
-  </si>
-  <si>
-    <t>4x1G</t>
-  </si>
-  <si>
-    <t>création du dé 1</t>
-  </si>
-  <si>
-    <t>création du dé 2</t>
-  </si>
-  <si>
-    <t>création du système de choix d'action</t>
-  </si>
-  <si>
-    <t>ce système permet de choisir la face que l'on souhaite mettre sur un de ses dés et l'achète si l'on a assez de ressources</t>
-  </si>
-  <si>
-    <t>création du système d'achat de faces</t>
-  </si>
-  <si>
-    <t>ce système fonctionnera après avec acheter une face et servira à la mettre sur le dé</t>
-  </si>
-  <si>
-    <t>création de l'option "demande de renfort"</t>
-  </si>
-  <si>
-    <t>création demande or pour marteau</t>
-  </si>
-  <si>
-    <t>il s'agit d'une option qui ne s'active que quand on a des renforts (les renforts sont notamment "les sabots d'argent")et permet d'activer l'effet d'une carte renfort, celle-ci se passe à chaque début de tour quand on a des renforts</t>
-  </si>
-  <si>
-    <t>il s'agit d'une methode demandant ce que l'on souhaite faire de l'or si l'on a un marteau qui n'est pas chargé à 100%, cette methode s'active à chaque fois que l'on obtient de l'or</t>
-  </si>
-  <si>
-    <t>création du système de forge</t>
-  </si>
-  <si>
-    <t>création d'une AI basique qui achetera un exploit lune si elle peut et forge sinon</t>
-  </si>
-  <si>
-    <t>ce système permet de choisir si l'on souhaite forger ou réaliser un exploit, ici il ne fera que forger</t>
-  </si>
-  <si>
-    <t>création de la face 3honour</t>
-  </si>
-  <si>
-    <t>création d'une AI honour</t>
-  </si>
-  <si>
-    <t>création de la face 2PdL+2honour</t>
-  </si>
-  <si>
-    <t>il s'agit d'une AI qui cherche uniquement à obtenir des faces honneur sur son dé et à les lancer à chaque tour en espérant tomber sur une face lui donnant de l'honour</t>
-  </si>
-  <si>
-    <t>il s'agit de la face 2PdL+2honour se trouvant dans le bassin à 12G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t>1honour</t>
-  </si>
-  <si>
-    <t>création de la face 1honour</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face permettant d'obtenir 1honour elle se trouve sur le dé numéro 2 de base</t>
-  </si>
-  <si>
-    <t>Il s'agit d'un dé possédant 4 faces à 1G, une face à 1PdL et une face à 1 honour</t>
-  </si>
-  <si>
-    <t>création de la face 4honour</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face dans le bassin à 12G permettant quand elle est roll sur le dé d'obtenir +4 honour</t>
-  </si>
-  <si>
-    <t>création de la face 3G ou 2honour</t>
-  </si>
-  <si>
-    <t>Il s'agit d'une face dans le bassin à 5G permettant quand elle est roll sur le dé d'obtenir 3gold ou 2 honour</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face dans le bassin à 8G permettant d'obtenir 3 honour</t>
-  </si>
-  <si>
     <t>à chaque fois que vous avez
  de l'or vous choisissez si 
 vous le gardez ou le mettez
  dans le marteau à 15G vous
- avez 10honour puis vous 
+ avez 10honor puis vous 
 pouvez recommencer pour 
-15honour et le marteau est 
+15honor et le marteau est 
 détruit</t>
-  </si>
-  <si>
-    <t>0honour</t>
-  </si>
-  <si>
-    <t>2honour</t>
-  </si>
-  <si>
-    <t>6honour</t>
-  </si>
-  <si>
-    <t>3G ou 2honour</t>
-  </si>
-  <si>
-    <t>12honour</t>
-  </si>
-  <si>
-    <t>4honour</t>
-  </si>
-  <si>
-    <t>8honour</t>
-  </si>
-  <si>
-    <t>26honour</t>
-  </si>
-  <si>
-    <t>3honour</t>
-  </si>
-  <si>
-    <t>3G=4honour</t>
-  </si>
-  <si>
-    <t>14honour</t>
-  </si>
-  <si>
-    <t>10honour</t>
-  </si>
-  <si>
-    <t>2honour+2PdL</t>
-  </si>
-  <si>
-    <t>Création d'une classe joueur qui comportera quatres variables gold,honour,PdL,PdS avec leur getter adder et remover</t>
-  </si>
-  <si>
-    <t>1PdS</t>
-  </si>
-  <si>
-    <t>création de la face PdS</t>
-  </si>
-  <si>
-    <t>Il s'agit d'une face étant dans un bassin à 3G et qui, quand elle est obtenue en lancant le dé donne une PdS</t>
-  </si>
-  <si>
-    <t>ce bassin sert à contenir les objets coutant 3G ici il contiendra des faces donnant une PdS</t>
-  </si>
-  <si>
-    <t>il s'agit d'un dé possédant 5 faces à 1G et une face à 1PdS</t>
-  </si>
-  <si>
-    <t>création d'une face 2PdS</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face permettant d'obtenir 2PdS se trouvant dans le bassin à 8G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t>création d'une AI PdS</t>
-  </si>
-  <si>
-    <t>Il s'agit d'une AI qui chechera à mettre le plus de PdS possible sur ses dés puis dès que possible acheter les objets les plus cher avec les PdS</t>
-  </si>
-  <si>
-    <t>création d'une face 1honour+1PdS</t>
-  </si>
-  <si>
-    <t>Il s'agit d'une face produisant 1honour +1PdS quand on tombe sur elle, elle se situe dans le bassin à 4G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t>création d'une face 1G ou 1PdS ou 1PdL</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face produisant soit 1G soit 1PdS ou alors 1PdL quand on tombe sur elle, elle se situe dans le bassin à 4G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t>création d'une face 1G+1PdS+1PdL+1honour</t>
-  </si>
-  <si>
-    <t>création d'une face 2PdS ou 2PdL ou 2G</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face produisant soit 2PdS soit 2PdL soit 2G, elle se situe dans le bassin à12G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t>Il s'agit d'une AI qui cherchera à obtenir le plus de ressource produite par face de son dé, avec ses PdS/PdL il achetera l'objet coutant le plus de la somme de ces deux pierres</t>
-  </si>
-  <si>
-    <t>http://jeuxstrategie1.free.fr/jeu_dice_forge/guide.PdS</t>
   </si>
   <si>
     <t>augmente vos réserves 
 maximales de +4G +3PdL 
-+3PdS pour chaque chest 
++3PdF pour chaque chest 
 acquis</t>
   </si>
   <si>
-    <t>4G/1PdS</t>
-  </si>
-  <si>
-    <t>6G/2G+1PdL/1honour+1PdS/
-1G ou 1PdS ou 1PdL</t>
-  </si>
-  <si>
-    <t>2PdS/3honour</t>
-  </si>
-  <si>
-    <t>4honour/1G+1PdS+1PdL+1honour
-/2PdS ou 2 PdL ou 2G
-/2honour+2PdL</t>
-  </si>
-  <si>
-    <t>2PdS</t>
-  </si>
-  <si>
-    <t>5PdL+5PdS</t>
-  </si>
-  <si>
-    <t>1G ou 1PdS ou 1PdL</t>
-  </si>
-  <si>
-    <t>1honour+1PdS</t>
-  </si>
-  <si>
-    <t>3PdS</t>
-  </si>
-  <si>
-    <t>4PdS</t>
-  </si>
-  <si>
-    <t>5PdS</t>
-  </si>
-  <si>
-    <t>1G+1PdS+1PdL+1honour</t>
-  </si>
-  <si>
-    <t>6PdS</t>
-  </si>
-  <si>
-    <t>2PdS ou 2PdL ou 2G</t>
+    <t>Création d'une classe joueur qui comportera quatres variables gold,honor,PdL,PdF avec leur getter adder et remover</t>
+  </si>
+  <si>
+    <t>Stéphane</t>
+  </si>
+  <si>
+    <t>création de dé</t>
+  </si>
+  <si>
+    <t>création d'une face 1G</t>
+  </si>
+  <si>
+    <t>création d'une face permettant d'obtenir 1gold, cette dernière devra être mise sur un dé pour être utilisée</t>
+  </si>
+  <si>
+    <t>DÉ 1</t>
+  </si>
+  <si>
+    <t>DÉ 2</t>
+  </si>
+  <si>
+    <t>1honor</t>
+  </si>
+  <si>
+    <t>BASSIN</t>
+  </si>
+  <si>
+    <t>1 à 2G</t>
+  </si>
+  <si>
+    <t>2 à 3G</t>
+  </si>
+  <si>
+    <t>3 à 4G</t>
+  </si>
+  <si>
+    <t>4 à 5G</t>
+  </si>
+  <si>
+    <t>5 à 6G</t>
+  </si>
+  <si>
+    <t>6 à 8G</t>
+  </si>
+  <si>
+    <t>7 à 12G</t>
+  </si>
+  <si>
+    <t>création d'une classe dice qui sera utilisable par chaque joueur et qui retournera un résultat entre 1 et 6 qui, plus tard, sera le numéro de la face qu'il aura obtenu (objet qui contiendra les objets faces)</t>
+  </si>
+  <si>
+    <t>création d'une AI basique qui fonctionnera sur du random.</t>
+  </si>
+  <si>
+    <t>création d'une face PdL</t>
+  </si>
+  <si>
+    <t>Il s'agit d'un exploit(carte dans le tableau ci-dessous) récompensant le joueur contre certaines ressources, durant cette slice on ne créera qu'un seul exploit demandant UNE PdL</t>
+  </si>
+  <si>
+    <t>création d'exploit(carte), marteau</t>
+  </si>
+  <si>
+    <t>création de l'exploit, chest</t>
+  </si>
+  <si>
+    <t>Création de l'exploit qui est décrit dans le tableau si dessous nommé chest, il sera sur la même ile que "marteau"</t>
+  </si>
+  <si>
+    <t>création de la face PdF</t>
+  </si>
+  <si>
+    <t>Il s'agit d'une face étant dans un bassin à 3G et qui, quand elle est obtenue en lancant le dé donne une PdF</t>
+  </si>
+  <si>
+    <t>Ile</t>
+  </si>
+  <si>
+    <t>1,lune</t>
+  </si>
+  <si>
+    <t>1lune</t>
+  </si>
+  <si>
+    <t>2,lune</t>
+  </si>
+  <si>
+    <t>3,lune</t>
+  </si>
+  <si>
+    <t>4,lune+soleil</t>
+  </si>
+  <si>
+    <t>1,soleil</t>
+  </si>
+  <si>
+    <t>2,soleil</t>
+  </si>
+  <si>
+    <t>3,soleil</t>
+  </si>
+  <si>
+    <t>création de l'ile 1,soleil</t>
+  </si>
+  <si>
+    <t>création de l'ile 1,lune</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'ile se trouvant en dessous de celle 1,lune et possédant deux exploit,"L'ancien" et "Les herbes folles"</t>
+  </si>
+  <si>
+    <t>Il s'agit d'un élément contenant plusieurs exploits, de plus deux joueurs ne peuvent pas être tout les deux sur une même ile, celui qui est arrivé en premier est renvoyé au spawn et peut relancer ses dés (faveur des dieux), durant cette slice on ne créera qu'une seule ile. la première ile créée sera l'ile 1,lune. cette ile possède deux exploit "marteau" et "chest"</t>
+  </si>
+  <si>
+    <t>création de l'exploit "L'ancien"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "L'ancien" décrit dans le tableau ci-dessous</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Les herbes folles"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "Les herbes folles" décrit dans le tableau ci-dessous</t>
+  </si>
+  <si>
+    <t>amelioration de l'AI pour qu'il y en ait une qui cherche à avoir le plus d'honneur via l'argent, strat marteau + ancien</t>
+  </si>
+  <si>
+    <t>l'AI developpée va chercher à réaliser la stratégie reposant sur l'argent où elle cherche à avoir le plus d'or obtenu sur ses dés, puis elle achete des anciens et enfin des marteaux, dès qu'elle a suffisament d'or à donner à ses anciens pour le tour suivant, elle donne tout son or aux marteaux.</t>
+  </si>
+  <si>
+    <t>création du bassin à 2G</t>
+  </si>
+  <si>
+    <t>il s'agit d'un objet possédant un nombre de case égal au nombre de joueur et possédant pour chaque bassin des faces spécifiques, le bassin a un prix pour acheter une face et on ne peut pas acheter durant le même tour deux faces du même bassin ce bassin possédera uniquement des objets coutant 2G, ici le seul objet créer à 2G est la face donnant 3G</t>
+  </si>
+  <si>
+    <t>création d'une face 3G</t>
+  </si>
+  <si>
+    <t>cette face ira dans le bassin à 2G</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face étant dans un bassin à 2G et qui, quand elle est obtenue en lancant le dé donne une PdL, elle se trouve dans le bassin à 2G</t>
+  </si>
+  <si>
+    <t>création du bassin à 3G</t>
+  </si>
+  <si>
+    <t>ce bassin sert à contenir les objets coutant 3G ici il contiendra des faces donnant une PdF</t>
+  </si>
+  <si>
+    <t>3G/1PdL</t>
+  </si>
+  <si>
+    <t>4G/1PdF</t>
+  </si>
+  <si>
+    <t>6G/2G+1PdL/1honor+1PdF/
+1G ou 1PdF ou 1PdL</t>
+  </si>
+  <si>
+    <t>2PdF/3honor</t>
+  </si>
+  <si>
+    <t>4honor/1G+1PdF+1PdL+1honor
+/2PdF ou 2 PdL ou 2G
+/2honor+2PdL</t>
+  </si>
+  <si>
+    <t>création de la face 4honor</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face dans le bassin à 12G permettant quand elle est roll sur le dé d'obtenir +4 honor</t>
+  </si>
+  <si>
+    <t>création de la face 3honor</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face dans le bassin à 8G permettant d'obtenir 3 honor</t>
+  </si>
+  <si>
+    <t>création d'une AI honor</t>
+  </si>
+  <si>
+    <t>3G ou 2honor</t>
+  </si>
+  <si>
+    <t>création de la face 3G ou 2honor</t>
+  </si>
+  <si>
+    <t>Il s'agit d'une face dans le bassin à 5G permettant quand elle est roll sur le dé d'obtenir 3gold ou 2 honor</t>
+  </si>
+  <si>
+    <t>il s'agit d'une AI qui cherche uniquement à obtenir des faces honneur sur son dé et à les lancer à chaque tour en espérant tomber sur une face lui donnant de l'honor</t>
+  </si>
+  <si>
+    <t>création de l'ile 2,lune</t>
+  </si>
+  <si>
+    <t>création de l'ile 3,lune</t>
+  </si>
+  <si>
+    <t>CARTE/EXPLOIT</t>
+  </si>
+  <si>
+    <t>il s'agit de la deuxième ile de la partie lune du plateau elle comporte deux exploits "Les sabots d'argent" et "Les satyres"</t>
+  </si>
+  <si>
+    <t>il s'agit de l'exploit "Les sabots d'argent" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,lune</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Les sabots d'argent"</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Les satyres"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "Les satyres" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,lune</t>
+  </si>
+  <si>
+    <t>il s'agit de la troisième ile de la partie lune du plateau elle comporte deux exploits "Le passeur" et "Le casque d'invisibilité"</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Le passeur"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "Le passeur" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,lune</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Le casque d'invisibilité"</t>
+  </si>
+  <si>
+    <t>il s'agit de l'exploit "Le casque d'invisibilité" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,lune</t>
+  </si>
+  <si>
+    <t>création du bassin à 12G</t>
+  </si>
+  <si>
+    <t>il s'agit du bassin à 12G décrit dans le tableau ci-dessous</t>
+  </si>
+  <si>
+    <t>création du bassin à 5G</t>
+  </si>
+  <si>
+    <t>Il s'agit du bassin à 5G décrit dans le tableau ci-dessous</t>
+  </si>
+  <si>
+    <t>création du bassin à 8G</t>
+  </si>
+  <si>
+    <t>il s'agit du bassin à 8G décrit dans le tableau ci-dessous</t>
+  </si>
+  <si>
+    <t>création de la face 2PdL</t>
+  </si>
+  <si>
+    <t>Il s'agit de la face 2PdL se trouvant dans le bassin à 6G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">création du bassin 6G </t>
+  </si>
+  <si>
+    <t>il s'agit du bassin 6G décrit dans le tableau ci-dessous</t>
+  </si>
+  <si>
+    <t>création de la face 2PdL+2honor</t>
+  </si>
+  <si>
+    <t>il s'agit de la face 2PdL+2honor se trouvant dans le bassin à 12G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t>création d'une AI PdL</t>
+  </si>
+  <si>
+    <t>Il s'agit d'une AI qui cherchera à obtenir sur son dé un maximum de face lui donnant des PdL puis sur les iles elle achetera l'objet coutant le plus de PdL dès qu'elle le peut</t>
+  </si>
+  <si>
+    <t>création d'une face 2PdF</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face permettant d'obtenir 2PdF se trouvant dans le bassin à 8G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t>création de l'ile 2,soleil</t>
+  </si>
+  <si>
+    <t>Il s'agit de la deuxième ile de la partie soleil du plateau elle comporte deux exploits "Les ailes de la gardienne" et "Le minotaure"</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Les ailes de la gardienne"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "Les ailes de la gardienne" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,soleil</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Le minotaure"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "Le minotaure" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,soleil</t>
+  </si>
+  <si>
+    <t>création de l'ile 3,soleil</t>
+  </si>
+  <si>
+    <t>Il s'agit de la troisième ile de la partie soleil du plateau elle comporte deux exploits "La méduse" et "Le miroir abyssal"</t>
+  </si>
+  <si>
+    <t>Le miroir abyssal</t>
+  </si>
+  <si>
+    <t>création de l'exploit "La méduse"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "La méduse" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,soleil</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Le miroir abyssal"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "Le miroir abyssal" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,soleil</t>
+  </si>
+  <si>
+    <t>création d'une AI PdF</t>
+  </si>
+  <si>
+    <t>Il s'agit d'une AI qui chechera à mettre le plus de PdF possible sur ses dés puis dès que possible acheter les objets les plus cher avec les PdF</t>
+  </si>
+  <si>
+    <t>création d'une face 2G +1PdL</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face produisant 2G + 1PdL quand on tombe sur elle, elle se situe dans le bassin à 4G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t>création d'une face 1honor+1PdF</t>
+  </si>
+  <si>
+    <t>création d'une face 1G ou 1PdF ou 1PdL</t>
+  </si>
+  <si>
+    <t>Il s'agit d'une face produisant 1honor +1PdF quand on tombe sur elle, elle se situe dans le bassin à 4G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face produisant soit 1G soit 1PdF ou alors 1PdL quand on tombe sur elle, elle se situe dans le bassin à 4G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t>création d'une face 1G+1PdF+1PdL+1honor</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face produisant un de toute les ressources, elle se situe dans le bassin à 12G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t>création d'une face 2PdF ou 2PdL ou 2G</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face produisant soit 2PdF soit 2PdL soit 2G, elle se situe dans le bassin à12G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t>création de l'ile 4,lune+soleil</t>
+  </si>
+  <si>
+    <t>Il s'agit de la quatrième ile des deux parcours lune et soleil, elle comporte trois exploits "La pince", "L'Hydre" et "L'énigme"</t>
+  </si>
+  <si>
+    <t>création de l'exploit "La pince"</t>
+  </si>
+  <si>
+    <t>création de l'exploit "L'Hydre"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "La pince" qui est décrit dans le tableau ci-dessous, il se trouve sur l'ile 4,lune+soleil, partie lune</t>
+  </si>
+  <si>
+    <t>il s'agit de l'exploit "L'Hydre" qui est décrit dans le tableau ci-dessous, il se trouve sur l'ile 4,lune+soleil,partie centrale</t>
+  </si>
+  <si>
+    <t>création de l'exploit "L'énigme"</t>
+  </si>
+  <si>
+    <t>il s'agit de l'exploit "L'énigme" qui est décrit dans letableau ci-dessous, il se trouve sur l'ile 4,lune+soleil, partie soleil</t>
+  </si>
+  <si>
+    <t>création d'une AI multi-ressources</t>
+  </si>
+  <si>
+    <t>Il s'agit d'une AI qui cherchera à obtenir le plus de ressource produite par face de son dé, avec ses PdF/PdL il achetera l'objet coutant le plus de la somme de ces deux pierres</t>
+  </si>
+  <si>
+    <t>5x1G</t>
+  </si>
+  <si>
+    <t>4x1G</t>
+  </si>
+  <si>
+    <t>création de la face 1honor</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face permettant d'obtenir 1honor elle se trouve sur le dé numéro 2 de base</t>
+  </si>
+  <si>
+    <t>création du dé 1</t>
+  </si>
+  <si>
+    <t>il s'agit d'un dé possédant 5 faces à 1G et une face à 1PdF</t>
+  </si>
+  <si>
+    <t>création du dé 2</t>
+  </si>
+  <si>
+    <t>Il s'agit d'un dé possédant 4 faces à 1G, une face à 1PdL et une face à 1 honor</t>
+  </si>
+  <si>
+    <t>création du système de choix d'action</t>
+  </si>
+  <si>
+    <t>ce système permet de choisir si l'on souhaite forge ou réaliser un exploit, ici il ne fera que forger</t>
+  </si>
+  <si>
+    <t>création du système de craft</t>
+  </si>
+  <si>
+    <t>ce système permet de choisir la face que l'on souhaite mettre sur un de ses dés et l'achète si l'on a assez de ressources</t>
+  </si>
+  <si>
+    <t>création du système d'achat de faces</t>
+  </si>
+  <si>
+    <t>ce système fonctionnera après avec acheter une face et servira à la mettre sur le dé</t>
+  </si>
+  <si>
+    <t>création de l'option "demande de renfort"</t>
+  </si>
+  <si>
+    <t>création demande or pour marteau</t>
+  </si>
+  <si>
+    <t>il s'agit d'une option qui ne s'active que quand on a des renforts (les renforts sont notamment "les sabots d'argent")et permet d'activer l'effet d'une carte renfort, celle-ci se passe à chaque début de tour quand on a des renforts</t>
+  </si>
+  <si>
+    <t>il s'agit d'une methode demandant ce que l'on souhaite faire de l'or si l'on a un marteau qui n'est pas chargé à 100%, cette methode s'active à chaque fois que l'on obtient de l'or</t>
   </si>
 </sst>
 </file>
@@ -892,7 +892,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1190,25 +1190,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07200E0C-4973-414C-A209-F8996EA50DD1}">
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.1640625" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="24.1640625" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30" customWidth="1"/>
-    <col min="12" max="12" width="22.5" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1240,13 +1240,13 @@
         <v>9</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1254,10 +1254,10 @@
         <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>197</v>
+        <v>84</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="7">
@@ -1276,49 +1276,47 @@
         <v>11</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="7">
-        <v>1</v>
-      </c>
+      <c r="F3" s="7"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="2"/>
       <c r="L3" s="13" t="s">
-        <v>198</v>
+        <v>45</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
-        <f>A3+1</f>
+        <f t="shared" ref="A4:A65" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -1326,24 +1324,24 @@
         <v>1</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
       <c r="J4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
-        <f t="shared" ref="A5:A10" si="0">A4+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -1355,16 +1353,16 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="206" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="206.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -1374,16 +1372,16 @@
       <c r="I6" s="6"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>158</v>
+        <v>221</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>168</v>
+        <v>222</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1393,16 +1391,16 @@
       <c r="I7" s="6"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>160</v>
+        <v>225</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>159</v>
+        <v>224</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -1412,16 +1410,16 @@
       <c r="I8" s="6"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>166</v>
+        <v>223</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>161</v>
+        <v>226</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1431,16 +1429,16 @@
       <c r="I9" s="6"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:13" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1450,16 +1448,16 @@
       <c r="I10" s="6"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:13" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <f>A10+1</f>
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1469,16 +1467,16 @@
       <c r="I11" s="6"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:13" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <f t="shared" ref="A12:A65" si="1">A11+1</f>
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>163</v>
+        <v>228</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>165</v>
+        <v>230</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1488,16 +1486,16 @@
       <c r="I12" s="6"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:13" ht="189" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="206.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>88</v>
+        <v>119</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1509,58 +1507,58 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:13" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>167</v>
+        <v>106</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>199</v>
+        <v>107</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>200</v>
+        <v>108</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -1572,16 +1570,16 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>201</v>
+        <v>134</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1591,16 +1589,16 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>175</v>
+        <v>215</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>176</v>
+        <v>216</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1610,16 +1608,16 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>156</v>
+        <v>217</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1629,16 +1627,16 @@
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>157</v>
+        <v>219</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>177</v>
+        <v>220</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -1648,16 +1646,16 @@
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -1669,16 +1667,16 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>91</v>
+        <v>122</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -1690,16 +1688,16 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -1711,16 +1709,16 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:10" ht="155" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="174.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>96</v>
+        <v>127</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -1732,16 +1730,16 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>178</v>
+        <v>140</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -1753,16 +1751,16 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>117</v>
+        <v>162</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -1772,16 +1770,16 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -1793,16 +1791,16 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>119</v>
+        <v>164</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -1814,16 +1812,16 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>182</v>
+        <v>143</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -1835,16 +1833,16 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>121</v>
+        <v>166</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -1854,16 +1852,16 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:10" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>170</v>
+        <v>144</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>172</v>
+        <v>148</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -1875,16 +1873,16 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
     </row>
-    <row r="32" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>123</v>
+        <v>168</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -1894,16 +1892,16 @@
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
     </row>
-    <row r="33" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>126</v>
+        <v>171</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -1913,13 +1911,13 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>173</v>
@@ -1932,16 +1930,16 @@
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
     </row>
-    <row r="35" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -1953,16 +1951,16 @@
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
     </row>
-    <row r="36" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>109</v>
+        <v>154</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -1974,16 +1972,16 @@
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
     </row>
-    <row r="37" spans="1:10" ht="138" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>162</v>
+        <v>227</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>164</v>
+        <v>229</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -1993,16 +1991,16 @@
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
     </row>
-    <row r="38" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -2014,16 +2012,16 @@
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
     </row>
-    <row r="39" spans="1:10" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>105</v>
+        <v>150</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -2035,16 +2033,16 @@
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
     </row>
-    <row r="40" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>114</v>
+        <v>159</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -2056,16 +2054,16 @@
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
     </row>
-    <row r="41" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -2077,16 +2075,16 @@
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
     </row>
-    <row r="42" spans="1:10" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>127</v>
+        <v>174</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>128</v>
+        <v>175</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -2098,16 +2096,16 @@
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
     </row>
-    <row r="43" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -2119,16 +2117,16 @@
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
     </row>
-    <row r="44" spans="1:10" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>129</v>
+        <v>178</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>130</v>
+        <v>179</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -2140,16 +2138,16 @@
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
     </row>
-    <row r="45" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>131</v>
+        <v>180</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>132</v>
+        <v>181</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -2161,16 +2159,16 @@
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
     </row>
-    <row r="46" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>133</v>
+        <v>182</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>134</v>
+        <v>183</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -2182,16 +2180,16 @@
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
     </row>
-    <row r="47" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>136</v>
+        <v>185</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
@@ -2203,16 +2201,16 @@
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
     </row>
-    <row r="48" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>138</v>
+        <v>187</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>139</v>
+        <v>188</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -2224,16 +2222,16 @@
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
     </row>
-    <row r="49" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>140</v>
+        <v>189</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>141</v>
+        <v>190</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
@@ -2245,16 +2243,16 @@
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
     </row>
-    <row r="50" spans="1:10" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
@@ -2266,16 +2264,16 @@
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
     </row>
-    <row r="51" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
@@ -2287,16 +2285,16 @@
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
     </row>
-    <row r="52" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
@@ -2308,16 +2306,16 @@
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
     </row>
-    <row r="53" spans="1:10" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -2329,16 +2327,16 @@
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
     </row>
-    <row r="54" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -2350,16 +2348,16 @@
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
     </row>
-    <row r="55" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
@@ -2371,16 +2369,16 @@
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
     </row>
-    <row r="56" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>145</v>
+        <v>203</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>146</v>
+        <v>204</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -2392,16 +2390,16 @@
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
     </row>
-    <row r="57" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>147</v>
+        <v>205</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>149</v>
+        <v>207</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
@@ -2413,16 +2411,16 @@
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
     </row>
-    <row r="58" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>150</v>
+        <v>208</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
@@ -2434,16 +2432,16 @@
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
     </row>
-    <row r="59" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>151</v>
+        <v>209</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>152</v>
+        <v>210</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
@@ -2455,16 +2453,16 @@
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
     </row>
-    <row r="60" spans="1:10" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>153</v>
+        <v>211</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
@@ -2476,7 +2474,7 @@
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
     </row>
-    <row r="61" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -2493,7 +2491,7 @@
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
     </row>
-    <row r="62" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -2510,7 +2508,7 @@
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
     </row>
-    <row r="63" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -2527,7 +2525,7 @@
       <c r="I63" s="6"/>
       <c r="J63" s="6"/>
     </row>
-    <row r="64" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -2544,7 +2542,7 @@
       <c r="I64" s="6"/>
       <c r="J64" s="6"/>
     </row>
-    <row r="65" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="7">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -2561,501 +2559,501 @@
       <c r="I65" s="6"/>
       <c r="J65" s="6"/>
     </row>
-    <row r="66" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B66" s="12"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="4" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="C69" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L69" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M69" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="121.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D69" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G69" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I69" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J69" s="4" t="s">
+      <c r="C70" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G70" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L69" s="4" t="s">
+      <c r="I70" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J70" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M70" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G71" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M69" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="130" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D70" s="2" t="s">
+      <c r="I71" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J71" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="M71" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E70" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="F70" s="2" t="s">
+      <c r="F72" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J72" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G70" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J70" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="L70" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="M70" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" ht="66" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J71" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="L71" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M71" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" ht="34" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="2" t="s">
+      <c r="C73" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J73" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="L73" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F72" s="2" t="s">
+      <c r="M73" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J74" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="G72" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="J72" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M72" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" ht="82" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J73" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="L73" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M73" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C74" s="2" t="s">
+      <c r="L74" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M74" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J74" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L74" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M74" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E75" s="2" t="s">
+      <c r="G75" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J75" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M75" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M76" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F75" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J75" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="L75" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="M75" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J76" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="L76" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="M76" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="F77" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>191</v>
+        <v>43</v>
       </c>
       <c r="I77" s="1"/>
       <c r="L77" s="2" t="s">
-        <v>192</v>
+        <v>72</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>198</v>
+        <v>45</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>193</v>
+        <v>48</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>184</v>
+        <v>47</v>
       </c>
       <c r="I78" s="1"/>
       <c r="L78" s="2" t="s">
-        <v>189</v>
+        <v>37</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>198</v>
+        <v>45</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>84</v>
+        <v>115</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>185</v>
+        <v>25</v>
       </c>
       <c r="I79" s="1"/>
       <c r="L79" s="2" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B80" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>221</v>
+        <v>52</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>223</v>
+        <v>53</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>189</v>
+        <v>37</v>
       </c>
       <c r="I80" s="1"/>
       <c r="L80" s="2" t="s">
-        <v>224</v>
+        <v>75</v>
       </c>
       <c r="M80" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="81" spans="2:13" ht="34" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="81" spans="2:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="2" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>225</v>
+        <v>55</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>190</v>
+        <v>38</v>
       </c>
       <c r="I81" s="1"/>
       <c r="L81" s="2" t="s">
-        <v>223</v>
+        <v>53</v>
       </c>
       <c r="M81" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="82" spans="2:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="82" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B82" s="2" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>226</v>
+        <v>58</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>194</v>
+        <v>59</v>
       </c>
       <c r="I82" s="1"/>
       <c r="L82" s="2" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="M82" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="83" spans="2:13" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" spans="2:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B83" s="2" t="s">
-        <v>137</v>
+        <v>186</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>227</v>
+        <v>60</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>195</v>
+        <v>62</v>
       </c>
       <c r="I83" s="1"/>
       <c r="L83" s="2" t="s">
-        <v>228</v>
+        <v>77</v>
       </c>
       <c r="M83" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="84" spans="2:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="84" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="2" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>229</v>
+        <v>64</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>83</v>
+        <v>114</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>195</v>
+        <v>62</v>
       </c>
       <c r="I84" s="1"/>
       <c r="L84" s="2" t="s">
-        <v>230</v>
+        <v>78</v>
       </c>
       <c r="M84" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="85" spans="2:13" ht="108" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="2:13" ht="108" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I85" s="1"/>
       <c r="L85" s="2" t="s">
-        <v>196</v>
+        <v>79</v>
       </c>
       <c r="M85" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="86" spans="2:13" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="87" spans="2:13" ht="75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" spans="2:13" ht="41.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="2:13" ht="75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="2:13" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#5 Small typing changes and minor slice reorganisation
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\PS5-18-19-DiceForge-EquipeG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bibi/Documents/PS5-18-19-DiceForge-EquipeG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9E4A4601-A912-43D9-9FF9-1B9BA37404F0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0CA6B7-75DE-E241-865D-BBCB26DBAC4F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" xr2:uid="{CDF5D2E8-3819-49DE-A1AD-AC0A83541AB5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16180" xr2:uid="{CDF5D2E8-3819-49DE-A1AD-AC0A83541AB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,9 +69,6 @@
     <t>créer une AI basique</t>
   </si>
   <si>
-    <t>http://jeuxstrategie1.free.fr/jeu_dice_forge/guide.pdf</t>
-  </si>
-  <si>
     <t>chest</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>oui</t>
   </si>
   <si>
-    <t>2honor</t>
-  </si>
-  <si>
     <t>Les satyres</t>
   </si>
   <si>
@@ -114,9 +108,6 @@
     <t>non</t>
   </si>
   <si>
-    <t>6honor</t>
-  </si>
-  <si>
     <t>Le passeur</t>
   </si>
   <si>
@@ -126,9 +117,6 @@
     <t>aucune</t>
   </si>
   <si>
-    <t>12honor</t>
-  </si>
-  <si>
     <t>Le casque d'invisibilité</t>
   </si>
   <si>
@@ -138,12 +126,6 @@
     <t>x3 une face du dé</t>
   </si>
   <si>
-    <t>4honor</t>
-  </si>
-  <si>
-    <t>8honor</t>
-  </si>
-  <si>
     <t>6PdL</t>
   </si>
   <si>
@@ -156,24 +138,9 @@
     <t>L'Hydre</t>
   </si>
   <si>
-    <t>26honor</t>
-  </si>
-  <si>
     <t>L'ancien</t>
   </si>
   <si>
-    <t>1PdF</t>
-  </si>
-  <si>
-    <t>5PdL+5PdF</t>
-  </si>
-  <si>
-    <t>0honor</t>
-  </si>
-  <si>
-    <t>3G=4honor</t>
-  </si>
-  <si>
     <t>Les herbes folles</t>
   </si>
   <si>
@@ -183,16 +150,7 @@
     <t>Les ailes de la gardienne</t>
   </si>
   <si>
-    <t>2PdF</t>
-  </si>
-  <si>
-    <t>1G ou 1PdF ou 1PdL</t>
-  </si>
-  <si>
     <t>Le minotaure</t>
-  </si>
-  <si>
-    <t>3PdF</t>
   </si>
   <si>
     <t>tlm lance les dés et retire 
@@ -200,15 +158,6 @@
   </si>
   <si>
     <t>La méduse</t>
-  </si>
-  <si>
-    <t>4PdF</t>
-  </si>
-  <si>
-    <t>14honor</t>
-  </si>
-  <si>
-    <t>5PdF</t>
   </si>
   <si>
     <t>forge une face sur son dé
@@ -216,15 +165,9 @@
 résultat du dé d'un adversaire</t>
   </si>
   <si>
-    <t>10honor</t>
-  </si>
-  <si>
     <t>L'énigme</t>
   </si>
   <si>
-    <t>6PdF</t>
-  </si>
-  <si>
     <t>relance 4 fois UN dé</t>
   </si>
   <si>
@@ -246,28 +189,13 @@
     <t>8G</t>
   </si>
   <si>
-    <t>3honor</t>
-  </si>
-  <si>
     <t>12G</t>
   </si>
   <si>
     <t>2G+1PdL</t>
   </si>
   <si>
-    <t>1honor+1PdF</t>
-  </si>
-  <si>
     <t>5G</t>
-  </si>
-  <si>
-    <t>1G+1PdF+1PdL+1honor</t>
-  </si>
-  <si>
-    <t>2PdF ou 2PdL ou 2G</t>
-  </si>
-  <si>
-    <t>2honor+2PdL</t>
   </si>
   <si>
     <t>relance UN dé</t>
@@ -280,464 +208,536 @@
  reçoivent rien</t>
   </si>
   <si>
+    <t>Stéphane</t>
+  </si>
+  <si>
+    <t>création de dé</t>
+  </si>
+  <si>
+    <t>création d'une face 1G</t>
+  </si>
+  <si>
+    <t>création d'une face permettant d'obtenir 1gold, cette dernière devra être mise sur un dé pour être utilisée</t>
+  </si>
+  <si>
+    <t>DÉ 1</t>
+  </si>
+  <si>
+    <t>DÉ 2</t>
+  </si>
+  <si>
+    <t>BASSIN</t>
+  </si>
+  <si>
+    <t>1 à 2G</t>
+  </si>
+  <si>
+    <t>2 à 3G</t>
+  </si>
+  <si>
+    <t>3 à 4G</t>
+  </si>
+  <si>
+    <t>4 à 5G</t>
+  </si>
+  <si>
+    <t>5 à 6G</t>
+  </si>
+  <si>
+    <t>6 à 8G</t>
+  </si>
+  <si>
+    <t>7 à 12G</t>
+  </si>
+  <si>
+    <t>création d'une classe dice qui sera utilisable par chaque joueur et qui retournera un résultat entre 1 et 6 qui, plus tard, sera le numéro de la face qu'il aura obtenu (objet qui contiendra les objets faces)</t>
+  </si>
+  <si>
+    <t>création d'une face PdL</t>
+  </si>
+  <si>
+    <t>Il s'agit d'un exploit(carte dans le tableau ci-dessous) récompensant le joueur contre certaines ressources, durant cette slice on ne créera qu'un seul exploit demandant UNE PdL</t>
+  </si>
+  <si>
+    <t>création d'exploit(carte), marteau</t>
+  </si>
+  <si>
+    <t>création de l'exploit, chest</t>
+  </si>
+  <si>
+    <t>Création de l'exploit qui est décrit dans le tableau si dessous nommé chest, il sera sur la même ile que "marteau"</t>
+  </si>
+  <si>
+    <t>Ile</t>
+  </si>
+  <si>
+    <t>1,lune</t>
+  </si>
+  <si>
+    <t>1lune</t>
+  </si>
+  <si>
+    <t>2,lune</t>
+  </si>
+  <si>
+    <t>3,lune</t>
+  </si>
+  <si>
+    <t>4,lune+soleil</t>
+  </si>
+  <si>
+    <t>1,soleil</t>
+  </si>
+  <si>
+    <t>2,soleil</t>
+  </si>
+  <si>
+    <t>3,soleil</t>
+  </si>
+  <si>
+    <t>création de l'ile 1,soleil</t>
+  </si>
+  <si>
+    <t>création de l'ile 1,lune</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'ile se trouvant en dessous de celle 1,lune et possédant deux exploit,"L'ancien" et "Les herbes folles"</t>
+  </si>
+  <si>
+    <t>Il s'agit d'un élément contenant plusieurs exploits, de plus deux joueurs ne peuvent pas être tout les deux sur une même ile, celui qui est arrivé en premier est renvoyé au spawn et peut relancer ses dés (faveur des dieux), durant cette slice on ne créera qu'une seule ile. la première ile créée sera l'ile 1,lune. cette ile possède deux exploit "marteau" et "chest"</t>
+  </si>
+  <si>
+    <t>création de l'exploit "L'ancien"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "L'ancien" décrit dans le tableau ci-dessous</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Les herbes folles"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "Les herbes folles" décrit dans le tableau ci-dessous</t>
+  </si>
+  <si>
+    <t>amelioration de l'AI pour qu'il y en ait une qui cherche à avoir le plus d'honneur via l'argent, strat marteau + ancien</t>
+  </si>
+  <si>
+    <t>l'AI developpée va chercher à réaliser la stratégie reposant sur l'argent où elle cherche à avoir le plus d'or obtenu sur ses dés, puis elle achete des anciens et enfin des marteaux, dès qu'elle a suffisament d'or à donner à ses anciens pour le tour suivant, elle donne tout son or aux marteaux.</t>
+  </si>
+  <si>
+    <t>création du bassin à 2G</t>
+  </si>
+  <si>
+    <t>il s'agit d'un objet possédant un nombre de case égal au nombre de joueur et possédant pour chaque bassin des faces spécifiques, le bassin a un prix pour acheter une face et on ne peut pas acheter durant le même tour deux faces du même bassin ce bassin possédera uniquement des objets coutant 2G, ici le seul objet créer à 2G est la face donnant 3G</t>
+  </si>
+  <si>
+    <t>création d'une face 3G</t>
+  </si>
+  <si>
+    <t>cette face ira dans le bassin à 2G</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face étant dans un bassin à 2G et qui, quand elle est obtenue en lancant le dé donne une PdL, elle se trouve dans le bassin à 2G</t>
+  </si>
+  <si>
+    <t>création du bassin à 3G</t>
+  </si>
+  <si>
+    <t>3G/1PdL</t>
+  </si>
+  <si>
+    <t>création de l'ile 2,lune</t>
+  </si>
+  <si>
+    <t>création de l'ile 3,lune</t>
+  </si>
+  <si>
+    <t>CARTE/EXPLOIT</t>
+  </si>
+  <si>
+    <t>il s'agit de la deuxième ile de la partie lune du plateau elle comporte deux exploits "Les sabots d'argent" et "Les satyres"</t>
+  </si>
+  <si>
+    <t>il s'agit de l'exploit "Les sabots d'argent" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,lune</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Les sabots d'argent"</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Les satyres"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "Les satyres" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,lune</t>
+  </si>
+  <si>
+    <t>il s'agit de la troisième ile de la partie lune du plateau elle comporte deux exploits "Le passeur" et "Le casque d'invisibilité"</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Le passeur"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "Le passeur" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,lune</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Le casque d'invisibilité"</t>
+  </si>
+  <si>
+    <t>il s'agit de l'exploit "Le casque d'invisibilité" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,lune</t>
+  </si>
+  <si>
+    <t>création du bassin à 12G</t>
+  </si>
+  <si>
+    <t>il s'agit du bassin à 12G décrit dans le tableau ci-dessous</t>
+  </si>
+  <si>
+    <t>création du bassin à 5G</t>
+  </si>
+  <si>
+    <t>Il s'agit du bassin à 5G décrit dans le tableau ci-dessous</t>
+  </si>
+  <si>
+    <t>création du bassin à 8G</t>
+  </si>
+  <si>
+    <t>il s'agit du bassin à 8G décrit dans le tableau ci-dessous</t>
+  </si>
+  <si>
+    <t>création de la face 2PdL</t>
+  </si>
+  <si>
+    <t>Il s'agit de la face 2PdL se trouvant dans le bassin à 6G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">création du bassin 6G </t>
+  </si>
+  <si>
+    <t>il s'agit du bassin 6G décrit dans le tableau ci-dessous</t>
+  </si>
+  <si>
+    <t>création d'une AI PdL</t>
+  </si>
+  <si>
+    <t>Il s'agit d'une AI qui cherchera à obtenir sur son dé un maximum de face lui donnant des PdL puis sur les iles elle achetera l'objet coutant le plus de PdL dès qu'elle le peut</t>
+  </si>
+  <si>
+    <t>création de l'ile 2,soleil</t>
+  </si>
+  <si>
+    <t>Il s'agit de la deuxième ile de la partie soleil du plateau elle comporte deux exploits "Les ailes de la gardienne" et "Le minotaure"</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Les ailes de la gardienne"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "Les ailes de la gardienne" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,soleil</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Le minotaure"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "Le minotaure" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,soleil</t>
+  </si>
+  <si>
+    <t>création de l'ile 3,soleil</t>
+  </si>
+  <si>
+    <t>Il s'agit de la troisième ile de la partie soleil du plateau elle comporte deux exploits "La méduse" et "Le miroir abyssal"</t>
+  </si>
+  <si>
+    <t>Le miroir abyssal</t>
+  </si>
+  <si>
+    <t>création de l'exploit "La méduse"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "La méduse" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,soleil</t>
+  </si>
+  <si>
+    <t>création de l'exploit "Le miroir abyssal"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "Le miroir abyssal" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,soleil</t>
+  </si>
+  <si>
+    <t>création d'une face 2G +1PdL</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face produisant 2G + 1PdL quand on tombe sur elle, elle se situe dans le bassin à 4G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face produisant un de toute les ressources, elle se situe dans le bassin à 12G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t>création de l'ile 4,lune+soleil</t>
+  </si>
+  <si>
+    <t>Il s'agit de la quatrième ile des deux parcours lune et soleil, elle comporte trois exploits "La pince", "L'Hydre" et "L'énigme"</t>
+  </si>
+  <si>
+    <t>création de l'exploit "La pince"</t>
+  </si>
+  <si>
+    <t>création de l'exploit "L'Hydre"</t>
+  </si>
+  <si>
+    <t>Il s'agit de l'exploit "La pince" qui est décrit dans le tableau ci-dessous, il se trouve sur l'ile 4,lune+soleil, partie lune</t>
+  </si>
+  <si>
+    <t>il s'agit de l'exploit "L'Hydre" qui est décrit dans le tableau ci-dessous, il se trouve sur l'ile 4,lune+soleil,partie centrale</t>
+  </si>
+  <si>
+    <t>création de l'exploit "L'énigme"</t>
+  </si>
+  <si>
+    <t>il s'agit de l'exploit "L'énigme" qui est décrit dans letableau ci-dessous, il se trouve sur l'ile 4,lune+soleil, partie soleil</t>
+  </si>
+  <si>
+    <t>création d'une AI multi-ressources</t>
+  </si>
+  <si>
+    <t>5x1G</t>
+  </si>
+  <si>
+    <t>4x1G</t>
+  </si>
+  <si>
+    <t>création du dé 1</t>
+  </si>
+  <si>
+    <t>création du dé 2</t>
+  </si>
+  <si>
+    <t>création du système de choix d'action</t>
+  </si>
+  <si>
+    <t>ce système permet de choisir la face que l'on souhaite mettre sur un de ses dés et l'achète si l'on a assez de ressources</t>
+  </si>
+  <si>
+    <t>création du système d'achat de faces</t>
+  </si>
+  <si>
+    <t>ce système fonctionnera après avec acheter une face et servira à la mettre sur le dé</t>
+  </si>
+  <si>
+    <t>création de l'option "demande de renfort"</t>
+  </si>
+  <si>
+    <t>création demande or pour marteau</t>
+  </si>
+  <si>
+    <t>il s'agit d'une option qui ne s'active que quand on a des renforts (les renforts sont notamment "les sabots d'argent")et permet d'activer l'effet d'une carte renfort, celle-ci se passe à chaque début de tour quand on a des renforts</t>
+  </si>
+  <si>
+    <t>il s'agit d'une methode demandant ce que l'on souhaite faire de l'or si l'on a un marteau qui n'est pas chargé à 100%, cette methode s'active à chaque fois que l'on obtient de l'or</t>
+  </si>
+  <si>
+    <t>création du système de forge</t>
+  </si>
+  <si>
+    <t>création d'une AI basique qui achetera un exploit lune si elle peut et forge sinon</t>
+  </si>
+  <si>
+    <t>ce système permet de choisir si l'on souhaite forger ou réaliser un exploit, ici il ne fera que forger</t>
+  </si>
+  <si>
+    <t>création de la face 3honour</t>
+  </si>
+  <si>
+    <t>création d'une AI honour</t>
+  </si>
+  <si>
+    <t>création de la face 2PdL+2honour</t>
+  </si>
+  <si>
+    <t>il s'agit d'une AI qui cherche uniquement à obtenir des faces honneur sur son dé et à les lancer à chaque tour en espérant tomber sur une face lui donnant de l'honour</t>
+  </si>
+  <si>
+    <t>il s'agit de la face 2PdL+2honour se trouvant dans le bassin à 12G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t>1honour</t>
+  </si>
+  <si>
+    <t>création de la face 1honour</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face permettant d'obtenir 1honour elle se trouve sur le dé numéro 2 de base</t>
+  </si>
+  <si>
+    <t>Il s'agit d'un dé possédant 4 faces à 1G, une face à 1PdL et une face à 1 honour</t>
+  </si>
+  <si>
+    <t>création de la face 4honour</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face dans le bassin à 12G permettant quand elle est roll sur le dé d'obtenir +4 honour</t>
+  </si>
+  <si>
+    <t>création de la face 3G ou 2honour</t>
+  </si>
+  <si>
+    <t>Il s'agit d'une face dans le bassin à 5G permettant quand elle est roll sur le dé d'obtenir 3gold ou 2 honour</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face dans le bassin à 8G permettant d'obtenir 3 honour</t>
+  </si>
+  <si>
     <t>à chaque fois que vous avez
  de l'or vous choisissez si 
 vous le gardez ou le mettez
  dans le marteau à 15G vous
- avez 10honor puis vous 
+ avez 10honour puis vous 
 pouvez recommencer pour 
-15honor et le marteau est 
+15honour et le marteau est 
 détruit</t>
+  </si>
+  <si>
+    <t>0honour</t>
+  </si>
+  <si>
+    <t>2honour</t>
+  </si>
+  <si>
+    <t>6honour</t>
+  </si>
+  <si>
+    <t>3G ou 2honour</t>
+  </si>
+  <si>
+    <t>12honour</t>
+  </si>
+  <si>
+    <t>4honour</t>
+  </si>
+  <si>
+    <t>8honour</t>
+  </si>
+  <si>
+    <t>26honour</t>
+  </si>
+  <si>
+    <t>3honour</t>
+  </si>
+  <si>
+    <t>3G=4honour</t>
+  </si>
+  <si>
+    <t>14honour</t>
+  </si>
+  <si>
+    <t>10honour</t>
+  </si>
+  <si>
+    <t>2honour+2PdL</t>
+  </si>
+  <si>
+    <t>Création d'une classe joueur qui comportera quatres variables gold,honour,PdL,PdS avec leur getter adder et remover</t>
+  </si>
+  <si>
+    <t>1PdS</t>
+  </si>
+  <si>
+    <t>création de la face PdS</t>
+  </si>
+  <si>
+    <t>Il s'agit d'une face étant dans un bassin à 3G et qui, quand elle est obtenue en lancant le dé donne une PdS</t>
+  </si>
+  <si>
+    <t>ce bassin sert à contenir les objets coutant 3G ici il contiendra des faces donnant une PdS</t>
+  </si>
+  <si>
+    <t>il s'agit d'un dé possédant 5 faces à 1G et une face à 1PdS</t>
+  </si>
+  <si>
+    <t>création d'une face 2PdS</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face permettant d'obtenir 2PdS se trouvant dans le bassin à 8G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t>création d'une AI PdS</t>
+  </si>
+  <si>
+    <t>Il s'agit d'une AI qui chechera à mettre le plus de PdS possible sur ses dés puis dès que possible acheter les objets les plus cher avec les PdS</t>
+  </si>
+  <si>
+    <t>création d'une face 1honour+1PdS</t>
+  </si>
+  <si>
+    <t>Il s'agit d'une face produisant 1honour +1PdS quand on tombe sur elle, elle se situe dans le bassin à 4G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t>création d'une face 1G ou 1PdS ou 1PdL</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face produisant soit 1G soit 1PdS ou alors 1PdL quand on tombe sur elle, elle se situe dans le bassin à 4G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t>création d'une face 1G+1PdS+1PdL+1honour</t>
+  </si>
+  <si>
+    <t>création d'une face 2PdS ou 2PdL ou 2G</t>
+  </si>
+  <si>
+    <t>il s'agit d'une face produisant soit 2PdS soit 2PdL soit 2G, elle se situe dans le bassin à12G décrit ci-dessous</t>
+  </si>
+  <si>
+    <t>Il s'agit d'une AI qui cherchera à obtenir le plus de ressource produite par face de son dé, avec ses PdS/PdL il achetera l'objet coutant le plus de la somme de ces deux pierres</t>
+  </si>
+  <si>
+    <t>http://jeuxstrategie1.free.fr/jeu_dice_forge/guide.PdS</t>
   </si>
   <si>
     <t>augmente vos réserves 
 maximales de +4G +3PdL 
-+3PdF pour chaque chest 
++3PdS pour chaque chest 
 acquis</t>
   </si>
   <si>
-    <t>Création d'une classe joueur qui comportera quatres variables gold,honor,PdL,PdF avec leur getter adder et remover</t>
-  </si>
-  <si>
-    <t>Stéphane</t>
-  </si>
-  <si>
-    <t>création de dé</t>
-  </si>
-  <si>
-    <t>création d'une face 1G</t>
-  </si>
-  <si>
-    <t>création d'une face permettant d'obtenir 1gold, cette dernière devra être mise sur un dé pour être utilisée</t>
-  </si>
-  <si>
-    <t>DÉ 1</t>
-  </si>
-  <si>
-    <t>DÉ 2</t>
-  </si>
-  <si>
-    <t>1honor</t>
-  </si>
-  <si>
-    <t>BASSIN</t>
-  </si>
-  <si>
-    <t>1 à 2G</t>
-  </si>
-  <si>
-    <t>2 à 3G</t>
-  </si>
-  <si>
-    <t>3 à 4G</t>
-  </si>
-  <si>
-    <t>4 à 5G</t>
-  </si>
-  <si>
-    <t>5 à 6G</t>
-  </si>
-  <si>
-    <t>6 à 8G</t>
-  </si>
-  <si>
-    <t>7 à 12G</t>
-  </si>
-  <si>
-    <t>création d'une classe dice qui sera utilisable par chaque joueur et qui retournera un résultat entre 1 et 6 qui, plus tard, sera le numéro de la face qu'il aura obtenu (objet qui contiendra les objets faces)</t>
-  </si>
-  <si>
-    <t>création d'une AI basique qui fonctionnera sur du random.</t>
-  </si>
-  <si>
-    <t>création d'une face PdL</t>
-  </si>
-  <si>
-    <t>Il s'agit d'un exploit(carte dans le tableau ci-dessous) récompensant le joueur contre certaines ressources, durant cette slice on ne créera qu'un seul exploit demandant UNE PdL</t>
-  </si>
-  <si>
-    <t>création d'exploit(carte), marteau</t>
-  </si>
-  <si>
-    <t>création de l'exploit, chest</t>
-  </si>
-  <si>
-    <t>Création de l'exploit qui est décrit dans le tableau si dessous nommé chest, il sera sur la même ile que "marteau"</t>
-  </si>
-  <si>
-    <t>création de la face PdF</t>
-  </si>
-  <si>
-    <t>Il s'agit d'une face étant dans un bassin à 3G et qui, quand elle est obtenue en lancant le dé donne une PdF</t>
-  </si>
-  <si>
-    <t>Ile</t>
-  </si>
-  <si>
-    <t>1,lune</t>
-  </si>
-  <si>
-    <t>1lune</t>
-  </si>
-  <si>
-    <t>2,lune</t>
-  </si>
-  <si>
-    <t>3,lune</t>
-  </si>
-  <si>
-    <t>4,lune+soleil</t>
-  </si>
-  <si>
-    <t>1,soleil</t>
-  </si>
-  <si>
-    <t>2,soleil</t>
-  </si>
-  <si>
-    <t>3,soleil</t>
-  </si>
-  <si>
-    <t>création de l'ile 1,soleil</t>
-  </si>
-  <si>
-    <t>création de l'ile 1,lune</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'ile se trouvant en dessous de celle 1,lune et possédant deux exploit,"L'ancien" et "Les herbes folles"</t>
-  </si>
-  <si>
-    <t>Il s'agit d'un élément contenant plusieurs exploits, de plus deux joueurs ne peuvent pas être tout les deux sur une même ile, celui qui est arrivé en premier est renvoyé au spawn et peut relancer ses dés (faveur des dieux), durant cette slice on ne créera qu'une seule ile. la première ile créée sera l'ile 1,lune. cette ile possède deux exploit "marteau" et "chest"</t>
-  </si>
-  <si>
-    <t>création de l'exploit "L'ancien"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "L'ancien" décrit dans le tableau ci-dessous</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Les herbes folles"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "Les herbes folles" décrit dans le tableau ci-dessous</t>
-  </si>
-  <si>
-    <t>amelioration de l'AI pour qu'il y en ait une qui cherche à avoir le plus d'honneur via l'argent, strat marteau + ancien</t>
-  </si>
-  <si>
-    <t>l'AI developpée va chercher à réaliser la stratégie reposant sur l'argent où elle cherche à avoir le plus d'or obtenu sur ses dés, puis elle achete des anciens et enfin des marteaux, dès qu'elle a suffisament d'or à donner à ses anciens pour le tour suivant, elle donne tout son or aux marteaux.</t>
-  </si>
-  <si>
-    <t>création du bassin à 2G</t>
-  </si>
-  <si>
-    <t>il s'agit d'un objet possédant un nombre de case égal au nombre de joueur et possédant pour chaque bassin des faces spécifiques, le bassin a un prix pour acheter une face et on ne peut pas acheter durant le même tour deux faces du même bassin ce bassin possédera uniquement des objets coutant 2G, ici le seul objet créer à 2G est la face donnant 3G</t>
-  </si>
-  <si>
-    <t>création d'une face 3G</t>
-  </si>
-  <si>
-    <t>cette face ira dans le bassin à 2G</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face étant dans un bassin à 2G et qui, quand elle est obtenue en lancant le dé donne une PdL, elle se trouve dans le bassin à 2G</t>
-  </si>
-  <si>
-    <t>création du bassin à 3G</t>
-  </si>
-  <si>
-    <t>ce bassin sert à contenir les objets coutant 3G ici il contiendra des faces donnant une PdF</t>
-  </si>
-  <si>
-    <t>3G/1PdL</t>
-  </si>
-  <si>
-    <t>4G/1PdF</t>
-  </si>
-  <si>
-    <t>6G/2G+1PdL/1honor+1PdF/
-1G ou 1PdF ou 1PdL</t>
-  </si>
-  <si>
-    <t>2PdF/3honor</t>
-  </si>
-  <si>
-    <t>4honor/1G+1PdF+1PdL+1honor
-/2PdF ou 2 PdL ou 2G
-/2honor+2PdL</t>
-  </si>
-  <si>
-    <t>création de la face 4honor</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face dans le bassin à 12G permettant quand elle est roll sur le dé d'obtenir +4 honor</t>
-  </si>
-  <si>
-    <t>création de la face 3honor</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face dans le bassin à 8G permettant d'obtenir 3 honor</t>
-  </si>
-  <si>
-    <t>création d'une AI honor</t>
-  </si>
-  <si>
-    <t>3G ou 2honor</t>
-  </si>
-  <si>
-    <t>création de la face 3G ou 2honor</t>
-  </si>
-  <si>
-    <t>Il s'agit d'une face dans le bassin à 5G permettant quand elle est roll sur le dé d'obtenir 3gold ou 2 honor</t>
-  </si>
-  <si>
-    <t>il s'agit d'une AI qui cherche uniquement à obtenir des faces honneur sur son dé et à les lancer à chaque tour en espérant tomber sur une face lui donnant de l'honor</t>
-  </si>
-  <si>
-    <t>création de l'ile 2,lune</t>
-  </si>
-  <si>
-    <t>création de l'ile 3,lune</t>
-  </si>
-  <si>
-    <t>CARTE/EXPLOIT</t>
-  </si>
-  <si>
-    <t>il s'agit de la deuxième ile de la partie lune du plateau elle comporte deux exploits "Les sabots d'argent" et "Les satyres"</t>
-  </si>
-  <si>
-    <t>il s'agit de l'exploit "Les sabots d'argent" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,lune</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Les sabots d'argent"</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Les satyres"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "Les satyres" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,lune</t>
-  </si>
-  <si>
-    <t>il s'agit de la troisième ile de la partie lune du plateau elle comporte deux exploits "Le passeur" et "Le casque d'invisibilité"</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Le passeur"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "Le passeur" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,lune</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Le casque d'invisibilité"</t>
-  </si>
-  <si>
-    <t>il s'agit de l'exploit "Le casque d'invisibilité" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,lune</t>
-  </si>
-  <si>
-    <t>création du bassin à 12G</t>
-  </si>
-  <si>
-    <t>il s'agit du bassin à 12G décrit dans le tableau ci-dessous</t>
-  </si>
-  <si>
-    <t>création du bassin à 5G</t>
-  </si>
-  <si>
-    <t>Il s'agit du bassin à 5G décrit dans le tableau ci-dessous</t>
-  </si>
-  <si>
-    <t>création du bassin à 8G</t>
-  </si>
-  <si>
-    <t>il s'agit du bassin à 8G décrit dans le tableau ci-dessous</t>
-  </si>
-  <si>
-    <t>création de la face 2PdL</t>
-  </si>
-  <si>
-    <t>Il s'agit de la face 2PdL se trouvant dans le bassin à 6G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">création du bassin 6G </t>
-  </si>
-  <si>
-    <t>il s'agit du bassin 6G décrit dans le tableau ci-dessous</t>
-  </si>
-  <si>
-    <t>création de la face 2PdL+2honor</t>
-  </si>
-  <si>
-    <t>il s'agit de la face 2PdL+2honor se trouvant dans le bassin à 12G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t>création d'une AI PdL</t>
-  </si>
-  <si>
-    <t>Il s'agit d'une AI qui cherchera à obtenir sur son dé un maximum de face lui donnant des PdL puis sur les iles elle achetera l'objet coutant le plus de PdL dès qu'elle le peut</t>
-  </si>
-  <si>
-    <t>création d'une face 2PdF</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face permettant d'obtenir 2PdF se trouvant dans le bassin à 8G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t>création de l'ile 2,soleil</t>
-  </si>
-  <si>
-    <t>Il s'agit de la deuxième ile de la partie soleil du plateau elle comporte deux exploits "Les ailes de la gardienne" et "Le minotaure"</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Les ailes de la gardienne"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "Les ailes de la gardienne" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,soleil</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Le minotaure"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "Le minotaure" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 2,soleil</t>
-  </si>
-  <si>
-    <t>création de l'ile 3,soleil</t>
-  </si>
-  <si>
-    <t>Il s'agit de la troisième ile de la partie soleil du plateau elle comporte deux exploits "La méduse" et "Le miroir abyssal"</t>
-  </si>
-  <si>
-    <t>Le miroir abyssal</t>
-  </si>
-  <si>
-    <t>création de l'exploit "La méduse"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "La méduse" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,soleil</t>
-  </si>
-  <si>
-    <t>création de l'exploit "Le miroir abyssal"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "Le miroir abyssal" qui est expliqué dans le tableau ci-dessous, il se situe sur l'ile 3,soleil</t>
-  </si>
-  <si>
-    <t>création d'une AI PdF</t>
-  </si>
-  <si>
-    <t>Il s'agit d'une AI qui chechera à mettre le plus de PdF possible sur ses dés puis dès que possible acheter les objets les plus cher avec les PdF</t>
-  </si>
-  <si>
-    <t>création d'une face 2G +1PdL</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face produisant 2G + 1PdL quand on tombe sur elle, elle se situe dans le bassin à 4G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t>création d'une face 1honor+1PdF</t>
-  </si>
-  <si>
-    <t>création d'une face 1G ou 1PdF ou 1PdL</t>
-  </si>
-  <si>
-    <t>Il s'agit d'une face produisant 1honor +1PdF quand on tombe sur elle, elle se situe dans le bassin à 4G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face produisant soit 1G soit 1PdF ou alors 1PdL quand on tombe sur elle, elle se situe dans le bassin à 4G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t>création d'une face 1G+1PdF+1PdL+1honor</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face produisant un de toute les ressources, elle se situe dans le bassin à 12G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t>création d'une face 2PdF ou 2PdL ou 2G</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face produisant soit 2PdF soit 2PdL soit 2G, elle se situe dans le bassin à12G décrit ci-dessous</t>
-  </si>
-  <si>
-    <t>création de l'ile 4,lune+soleil</t>
-  </si>
-  <si>
-    <t>Il s'agit de la quatrième ile des deux parcours lune et soleil, elle comporte trois exploits "La pince", "L'Hydre" et "L'énigme"</t>
-  </si>
-  <si>
-    <t>création de l'exploit "La pince"</t>
-  </si>
-  <si>
-    <t>création de l'exploit "L'Hydre"</t>
-  </si>
-  <si>
-    <t>Il s'agit de l'exploit "La pince" qui est décrit dans le tableau ci-dessous, il se trouve sur l'ile 4,lune+soleil, partie lune</t>
-  </si>
-  <si>
-    <t>il s'agit de l'exploit "L'Hydre" qui est décrit dans le tableau ci-dessous, il se trouve sur l'ile 4,lune+soleil,partie centrale</t>
-  </si>
-  <si>
-    <t>création de l'exploit "L'énigme"</t>
-  </si>
-  <si>
-    <t>il s'agit de l'exploit "L'énigme" qui est décrit dans letableau ci-dessous, il se trouve sur l'ile 4,lune+soleil, partie soleil</t>
-  </si>
-  <si>
-    <t>création d'une AI multi-ressources</t>
-  </si>
-  <si>
-    <t>Il s'agit d'une AI qui cherchera à obtenir le plus de ressource produite par face de son dé, avec ses PdF/PdL il achetera l'objet coutant le plus de la somme de ces deux pierres</t>
-  </si>
-  <si>
-    <t>5x1G</t>
-  </si>
-  <si>
-    <t>4x1G</t>
-  </si>
-  <si>
-    <t>création de la face 1honor</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face permettant d'obtenir 1honor elle se trouve sur le dé numéro 2 de base</t>
-  </si>
-  <si>
-    <t>création du dé 1</t>
-  </si>
-  <si>
-    <t>il s'agit d'un dé possédant 5 faces à 1G et une face à 1PdF</t>
-  </si>
-  <si>
-    <t>création du dé 2</t>
-  </si>
-  <si>
-    <t>Il s'agit d'un dé possédant 4 faces à 1G, une face à 1PdL et une face à 1 honor</t>
-  </si>
-  <si>
-    <t>création du système de choix d'action</t>
-  </si>
-  <si>
-    <t>ce système permet de choisir si l'on souhaite forge ou réaliser un exploit, ici il ne fera que forger</t>
-  </si>
-  <si>
-    <t>création du système de craft</t>
-  </si>
-  <si>
-    <t>ce système permet de choisir la face que l'on souhaite mettre sur un de ses dés et l'achète si l'on a assez de ressources</t>
-  </si>
-  <si>
-    <t>création du système d'achat de faces</t>
-  </si>
-  <si>
-    <t>ce système fonctionnera après avec acheter une face et servira à la mettre sur le dé</t>
-  </si>
-  <si>
-    <t>création de l'option "demande de renfort"</t>
-  </si>
-  <si>
-    <t>création demande or pour marteau</t>
-  </si>
-  <si>
-    <t>il s'agit d'une option qui ne s'active que quand on a des renforts (les renforts sont notamment "les sabots d'argent")et permet d'activer l'effet d'une carte renfort, celle-ci se passe à chaque début de tour quand on a des renforts</t>
-  </si>
-  <si>
-    <t>il s'agit d'une methode demandant ce que l'on souhaite faire de l'or si l'on a un marteau qui n'est pas chargé à 100%, cette methode s'active à chaque fois que l'on obtient de l'or</t>
+    <t>4G/1PdS</t>
+  </si>
+  <si>
+    <t>6G/2G+1PdL/1honour+1PdS/
+1G ou 1PdS ou 1PdL</t>
+  </si>
+  <si>
+    <t>2PdS/3honour</t>
+  </si>
+  <si>
+    <t>4honour/1G+1PdS+1PdL+1honour
+/2PdS ou 2 PdL ou 2G
+/2honour+2PdL</t>
+  </si>
+  <si>
+    <t>2PdS</t>
+  </si>
+  <si>
+    <t>5PdL+5PdS</t>
+  </si>
+  <si>
+    <t>1G ou 1PdS ou 1PdL</t>
+  </si>
+  <si>
+    <t>1honour+1PdS</t>
+  </si>
+  <si>
+    <t>3PdS</t>
+  </si>
+  <si>
+    <t>4PdS</t>
+  </si>
+  <si>
+    <t>5PdS</t>
+  </si>
+  <si>
+    <t>1G+1PdS+1PdL+1honour</t>
+  </si>
+  <si>
+    <t>6PdS</t>
+  </si>
+  <si>
+    <t>2PdS ou 2PdL ou 2G</t>
   </si>
 </sst>
 </file>
@@ -892,7 +892,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1190,25 +1190,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07200E0C-4973-414C-A209-F8996EA50DD1}">
   <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" customWidth="1"/>
+    <col min="12" max="12" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1240,13 +1240,13 @@
         <v>9</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1254,10 +1254,10 @@
         <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>84</v>
+        <v>197</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="7">
@@ -1276,47 +1276,51 @@
         <v>11</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>213</v>
+        <v>154</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
+      <c r="H3" s="9">
+        <v>43385</v>
+      </c>
+      <c r="I3" s="6"/>
       <c r="J3" s="2"/>
       <c r="L3" s="13" t="s">
-        <v>45</v>
+        <v>198</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
-        <f t="shared" ref="A4:A65" si="0">A3+1</f>
+        <f>A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -1324,24 +1328,24 @@
         <v>1</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
       <c r="J4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A5:A10" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -1353,16 +1357,16 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="206.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="206" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>128</v>
+        <v>97</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -1372,16 +1376,16 @@
       <c r="I6" s="6"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>221</v>
+        <v>158</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>222</v>
+        <v>168</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1391,16 +1395,16 @@
       <c r="I7" s="6"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:13" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>225</v>
+        <v>160</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>224</v>
+        <v>159</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -1410,16 +1414,16 @@
       <c r="I8" s="6"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>223</v>
+        <v>166</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>226</v>
+        <v>161</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
@@ -1429,16 +1433,16 @@
       <c r="I9" s="6"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:13" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1448,16 +1452,16 @@
       <c r="I10" s="6"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:13" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <f>A10+1</f>
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1467,16 +1471,16 @@
       <c r="I11" s="6"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:13" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <f t="shared" ref="A12:A65" si="1">A11+1</f>
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>228</v>
+        <v>163</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>230</v>
+        <v>165</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1486,16 +1490,16 @@
       <c r="I12" s="6"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:13" ht="206.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="189" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1507,58 +1511,58 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:13" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>106</v>
+        <v>167</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
     </row>
-    <row r="16" spans="1:13" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>107</v>
+        <v>199</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>108</v>
+        <v>200</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -1570,16 +1574,16 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>134</v>
+        <v>201</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1589,16 +1593,16 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>215</v>
+        <v>175</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>216</v>
+        <v>176</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1608,16 +1612,16 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>217</v>
+        <v>156</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1627,16 +1631,16 @@
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>219</v>
+        <v>157</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -1646,16 +1650,16 @@
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -1667,16 +1671,16 @@
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -1688,16 +1692,16 @@
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -1709,16 +1713,16 @@
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:10" ht="174.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="155" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -1730,16 +1734,16 @@
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>140</v>
+        <v>178</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>141</v>
+        <v>179</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -1751,16 +1755,16 @@
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>162</v>
+        <v>117</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>163</v>
+        <v>118</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -1770,16 +1774,16 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -1791,16 +1795,16 @@
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:10" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>164</v>
+        <v>119</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>165</v>
+        <v>120</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -1812,16 +1816,16 @@
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>142</v>
+        <v>169</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>143</v>
+        <v>182</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
@@ -1833,16 +1837,16 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:10" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>166</v>
+        <v>121</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>167</v>
+        <v>122</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
@@ -1852,16 +1856,16 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:10" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>144</v>
+        <v>170</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
@@ -1873,16 +1877,16 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
     </row>
-    <row r="32" spans="1:10" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>168</v>
+        <v>123</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>169</v>
+        <v>124</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -1892,16 +1896,16 @@
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
     </row>
-    <row r="33" spans="1:10" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>170</v>
+        <v>125</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>171</v>
+        <v>126</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -1911,13 +1915,13 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>173</v>
@@ -1930,16 +1934,16 @@
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
     </row>
-    <row r="35" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>149</v>
+        <v>104</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>152</v>
+        <v>107</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
@@ -1951,16 +1955,16 @@
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
     </row>
-    <row r="36" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>154</v>
+        <v>109</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>153</v>
+        <v>108</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
@@ -1972,16 +1976,16 @@
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
     </row>
-    <row r="37" spans="1:10" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="138" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>227</v>
+        <v>162</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>229</v>
+        <v>164</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -1991,16 +1995,16 @@
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
     </row>
-    <row r="38" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>155</v>
+        <v>110</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>156</v>
+        <v>111</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -2012,16 +2016,16 @@
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
     </row>
-    <row r="39" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>150</v>
+        <v>105</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>157</v>
+        <v>112</v>
       </c>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -2033,16 +2037,16 @@
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
     </row>
-    <row r="40" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>158</v>
+        <v>113</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -2054,16 +2058,16 @@
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
     </row>
-    <row r="41" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>160</v>
+        <v>115</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>161</v>
+        <v>116</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -2075,16 +2079,16 @@
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
     </row>
-    <row r="42" spans="1:10" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>174</v>
+        <v>127</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>175</v>
+        <v>128</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -2096,16 +2100,16 @@
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
     </row>
-    <row r="43" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>176</v>
+        <v>203</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -2117,16 +2121,16 @@
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
     </row>
-    <row r="44" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>178</v>
+        <v>129</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>179</v>
+        <v>130</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -2138,16 +2142,16 @@
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
     </row>
-    <row r="45" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>180</v>
+        <v>131</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>181</v>
+        <v>132</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -2159,16 +2163,16 @@
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
     </row>
-    <row r="46" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>182</v>
+        <v>133</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>183</v>
+        <v>134</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -2180,16 +2184,16 @@
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
     </row>
-    <row r="47" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>184</v>
+        <v>135</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>185</v>
+        <v>136</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
@@ -2201,16 +2205,16 @@
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
     </row>
-    <row r="48" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>187</v>
+        <v>138</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>188</v>
+        <v>139</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -2222,16 +2226,16 @@
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
     </row>
-    <row r="49" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>190</v>
+        <v>141</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
@@ -2243,16 +2247,16 @@
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
     </row>
-    <row r="50" spans="1:10" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
@@ -2264,16 +2268,16 @@
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
     </row>
-    <row r="51" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>193</v>
+        <v>142</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>194</v>
+        <v>143</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
@@ -2285,16 +2289,16 @@
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
     </row>
-    <row r="52" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>195</v>
+        <v>207</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="D52" s="6"/>
       <c r="E52" s="6"/>
@@ -2306,16 +2310,16 @@
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
     </row>
-    <row r="53" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -2327,16 +2331,16 @@
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
     </row>
-    <row r="54" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>200</v>
+        <v>144</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -2348,16 +2352,16 @@
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
     </row>
-    <row r="55" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <f t="shared" si="1"/>
         <v>54</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
@@ -2369,16 +2373,16 @@
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
     </row>
-    <row r="56" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>203</v>
+        <v>145</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>204</v>
+        <v>146</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="6"/>
@@ -2390,16 +2394,16 @@
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
     </row>
-    <row r="57" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>205</v>
+        <v>147</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>207</v>
+        <v>149</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="6"/>
@@ -2411,16 +2415,16 @@
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
     </row>
-    <row r="58" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <f t="shared" si="1"/>
         <v>57</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>206</v>
+        <v>148</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>208</v>
+        <v>150</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
@@ -2432,16 +2436,16 @@
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
     </row>
-    <row r="59" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <f t="shared" si="1"/>
         <v>58</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>209</v>
+        <v>151</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>210</v>
+        <v>152</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
@@ -2453,16 +2457,16 @@
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
     </row>
-    <row r="60" spans="1:10" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>211</v>
+        <v>153</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
@@ -2474,7 +2478,7 @@
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
     </row>
-    <row r="61" spans="1:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -2491,7 +2495,7 @@
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
     </row>
-    <row r="62" spans="1:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <f t="shared" si="1"/>
         <v>61</v>
@@ -2508,7 +2512,7 @@
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
     </row>
-    <row r="63" spans="1:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <f t="shared" si="1"/>
         <v>62</v>
@@ -2525,7 +2529,7 @@
       <c r="I63" s="6"/>
       <c r="J63" s="6"/>
     </row>
-    <row r="64" spans="1:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <f t="shared" si="1"/>
         <v>63</v>
@@ -2542,7 +2546,7 @@
       <c r="I64" s="6"/>
       <c r="J64" s="6"/>
     </row>
-    <row r="65" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <f t="shared" si="1"/>
         <v>64</v>
@@ -2559,501 +2563,501 @@
       <c r="I65" s="6"/>
       <c r="J65" s="6"/>
     </row>
-    <row r="66" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B66" s="12"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J69" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L69" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M69" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" ht="130" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J70" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="L70" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M70" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="66" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="69" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G69" s="4" t="s">
+      <c r="C71" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I69" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="J69" s="4" t="s">
+      <c r="D71" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I71" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="L69" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="M69" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="121.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C70" s="2" t="s">
+      <c r="J71" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M71" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="34" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E70" s="3" t="s">
+      <c r="C72" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J72" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M72" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="82" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J73" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="L73" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M73" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F70" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I70" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="J70" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="L70" s="2" t="s">
+      <c r="E74" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J74" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M74" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I75" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="M70" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E71" s="3" t="s">
+      <c r="J75" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="M75" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D76" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F71" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I71" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J71" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="L71" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="M71" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J72" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="M72" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="2" t="s">
+      <c r="E76" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F76" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G73" s="2" t="s">
+      <c r="G76" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="L76" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="M76" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I73" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="J73" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="L73" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M73" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J74" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="L74" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M74" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J75" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="L75" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M75" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J76" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="L76" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="M76" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F77" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>43</v>
+        <v>191</v>
       </c>
       <c r="I77" s="1"/>
       <c r="L77" s="2" t="s">
-        <v>72</v>
+        <v>192</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>45</v>
+        <v>198</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>48</v>
+        <v>193</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>47</v>
+        <v>184</v>
       </c>
       <c r="I78" s="1"/>
       <c r="L78" s="2" t="s">
-        <v>37</v>
+        <v>189</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>45</v>
+        <v>198</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="I79" s="1"/>
       <c r="L79" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>52</v>
+        <v>221</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>53</v>
+        <v>223</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>37</v>
+        <v>189</v>
       </c>
       <c r="I80" s="1"/>
       <c r="L80" s="2" t="s">
-        <v>75</v>
+        <v>224</v>
       </c>
       <c r="M80" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="81" spans="2:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="81" spans="2:13" ht="34" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>55</v>
+        <v>225</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>38</v>
+        <v>190</v>
       </c>
       <c r="I81" s="1"/>
       <c r="L81" s="2" t="s">
-        <v>53</v>
+        <v>223</v>
       </c>
       <c r="M81" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="82" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="82" spans="2:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>58</v>
+        <v>226</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>59</v>
+        <v>194</v>
       </c>
       <c r="I82" s="1"/>
       <c r="L82" s="2" t="s">
-        <v>145</v>
+        <v>187</v>
       </c>
       <c r="M82" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="83" spans="2:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="83" spans="2:13" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>186</v>
+        <v>137</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>60</v>
+        <v>227</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>62</v>
+        <v>195</v>
       </c>
       <c r="I83" s="1"/>
       <c r="L83" s="2" t="s">
-        <v>77</v>
+        <v>228</v>
       </c>
       <c r="M83" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="84" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="84" spans="2:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>64</v>
+        <v>229</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>62</v>
+        <v>195</v>
       </c>
       <c r="I84" s="1"/>
       <c r="L84" s="2" t="s">
-        <v>78</v>
+        <v>230</v>
       </c>
       <c r="M84" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="85" spans="2:13" ht="108" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="85" spans="2:13" ht="108" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I85" s="1"/>
       <c r="L85" s="2" t="s">
-        <v>79</v>
+        <v>196</v>
       </c>
       <c r="M85" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="86" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="2:13" ht="75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="2:13" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="86" spans="2:13" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="87" spans="2:13" ht="75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" spans="2:13" ht="41.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#4 ajout de toutes les acceptations pour les slices prévues actuellement
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bibi/Documents/PS5-18-19-DiceForge-EquipeG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stéphane\Documents\GitHub\PS5-18-19-DiceForge-EquipeG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2D254D-756B-0F48-BEA1-14D8EE29CCBC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="16185"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="253">
   <si>
     <t>Numéro</t>
   </si>
@@ -475,13 +474,7 @@
     <t>ce système fonctionnera après avec acheter une face et servira à la mettre sur le dé</t>
   </si>
   <si>
-    <t>création de l'option "demande de renfort"</t>
-  </si>
-  <si>
     <t>création demande or pour marteau</t>
-  </si>
-  <si>
-    <t>il s'agit d'une option qui ne s'active que quand on a des renforts (les renforts sont notamment "les sabots d'argent")et permet d'activer l'effet d'une carte renfort, celle-ci se passe à chaque début de tour quand on a des renforts</t>
   </si>
   <si>
     <t>il s'agit d'une methode demandant ce que l'on souhaite faire de l'or si l'on a un marteau qui n'est pas chargé à 100%, cette methode s'active à chaque fois que l'on obtient de l'or</t>
@@ -560,12 +553,6 @@
     <t>1PdS</t>
   </si>
   <si>
-    <t>création d'une face 2PdS</t>
-  </si>
-  <si>
-    <t>il s'agit d'une face permettant d'obtenir 2PdS se trouvant dans le bassin à 8G décrit ci-dessous</t>
-  </si>
-  <si>
     <t>création d'une AI PdS</t>
   </si>
   <si>
@@ -691,11 +678,137 @@
   <si>
     <t>Les variables du joueur changent correctement lors de l'utilisation des fonctions associées.</t>
   </si>
+  <si>
+    <t>Le bassin possède bien deux faces actuellement, toutes les faces dedans coutent 2G.</t>
+  </si>
+  <si>
+    <t>On propose de passer son tour, de forger ou de réaliser un exploit, ici seul forger réalise quelque chose, les autres casent passent le tour/arrête programme pour la case exploit</t>
+  </si>
+  <si>
+    <t>Quand on a accepté de forger, on choisit quelle face acheter, si l'on a assez d'argent, pour l'instant, on nous dit que l'on peut forger. On peut toujours annuler et retourner en arrière tant qu'on a pas acheté de face</t>
+  </si>
+  <si>
+    <t>Après que la face a été achetée on demande où il veut forger la face</t>
+  </si>
+  <si>
+    <t>Maintenant quand dans le système de choix d'action, quand on cliquera sur exploit on pourra aller sur l'ile 1,lune aucune action n'est encore possible en allant sur cette ile car elle ne possède pas d'exploit pour l'instant</t>
+  </si>
+  <si>
+    <t>quand on possède un marteau, à chaque fois que l'on obtient de l'or, on nous demande combien d'or on veut mettre sur la carte de l'exploit marteau</t>
+  </si>
+  <si>
+    <t>quand on se rend sur l'ile 1,lune on peut acheter un chest si l'on a une PdL</t>
+  </si>
+  <si>
+    <t>quand on se rend sur l'ile 1,lune on peut acheter un marteau si l'on a une PdL</t>
+  </si>
+  <si>
+    <t>on lance une centaines de fois l'AI et observe si elle gagne/perd contre celle qui lance uniquement son dé</t>
+  </si>
+  <si>
+    <t>le constructeur existe déjà mais on construira pour le jeu le bassin à 3G avec les faces adéquate, pour la vérification si ça fonctionne il suffit de voir si l'on peut bien les acheter et les craft sur nos dés</t>
+  </si>
+  <si>
+    <t>maintenant dans la partie exploit on peut choisir d'aller sur une autre ile, ici l'ile 1,soleil, où l'on ne peut rien faire pour l'instant à par s'y rendre</t>
+  </si>
+  <si>
+    <t>Si l'on a assez de PdS (ici 1PdS) on peut acheter "L'ancien" celui-ci ne rapportera que la récompense pour l'instant et pas son actif à chaque tour</t>
+  </si>
+  <si>
+    <t>création du système de renfort</t>
+  </si>
+  <si>
+    <t>à chaque début de tour si le joueur active possède une carte répétitive, on peut choisir si on l'active ou non</t>
+  </si>
+  <si>
+    <t>Si on a acheté "L'ancien" que c'est le début de notre tour on nous propose si on veut activer l'effet actif de "L'ancien" si on dit oui, il s'active, sinon on peut refuser et passer à son choix d'action pour son tour</t>
+  </si>
+  <si>
+    <t>Si l'on a assez de PdS (ici 1PdS) on peut acheter "Les herbes folles" ce qui nous fait obtenir 3gold et 3PdL, après avoir acheter "Les herbes folles" il suffit de vérifier si l'on a obtenu cet argent (dans la limite de la capacité de stockage maximal du joueur)</t>
+  </si>
+  <si>
+    <t>après avoir programmé l'AI on lance beaucoup de partie à la suite pour voir si l'AI argent -&gt; honor fonctionne bien</t>
+  </si>
+  <si>
+    <t>Il suffit d'acheter des faces dans ce bassin et voir si l'on a bien perdu 12G et obtenu la face sur le dé</t>
+  </si>
+  <si>
+    <t>Il suffit d'acheter des faces dans ce bassin et voir si l'on a bien perdu 5G et obtenu la face sur le dé</t>
+  </si>
+  <si>
+    <t>Il suffit d'acheter des faces dans ce bassin et voir si l'on a bien perdu 8G et obtenu la face sur le dé</t>
+  </si>
+  <si>
+    <t>Il suffit d'acheter l'h faces uniquement sur lancer tomber de ce d'une et voir AI d'on h bien perdu honour et obtenu la face sur lui fa</t>
+  </si>
+  <si>
+    <t>Il suffit d'acheter des faces le ce du et voir si l'on a bien perdu 6G et obtenu la face sur le dé</t>
+  </si>
+  <si>
+    <t>maintenant dans la partie exploit on peut choisir d'aller dans l'ile 2,lune</t>
+  </si>
+  <si>
+    <t>si l'on a assez de PdS on peut acheter l'exploit "Les sabots d'argent", pour vérifier si l'on a obtenu de l'honneur et si pendant la phase de renfort on peut activer "les sabots d'argent" alors "Les sabots d'argent" sont bien implémentés</t>
+  </si>
+  <si>
+    <t>Si l'on a assez de PdS on peut acheter l'exploit "Les satyres", quand il est acheté il faut vérifier si l'action des satyres décrite dans le tableau ci-dessous se lance</t>
+  </si>
+  <si>
+    <t>vérifier si l'on peut aller sur l'ile 3,lune</t>
+  </si>
+  <si>
+    <t>ajout sur l'ile 3,lune de l'exploit "Le passeur" quand cet exploit est acheté (si l'on a assez de PdL) son action décrite plus bas s'active et on obtient la récompense</t>
+  </si>
+  <si>
+    <t>Quand cet AI sera programmée on lancera des parties entre elles et les AI précedentes pour voir qui s'en sort le mieux</t>
+  </si>
+  <si>
+    <t>ajout sur l'ile 3,lune de l'exploit "Le casque d'invisibilité" quand cet exploit est acheté (si l'on a assez de PdL) son action décrite plus bas s'active et on obtient la récompense</t>
+  </si>
+  <si>
+    <t>vérifier si l'on peut aller sur l'ile 2,soleil</t>
+  </si>
+  <si>
+    <t>ajout à l'ile 2,soleil de l'exploit "Les ailes de la gardienne" quand ce dernier est acheté, durant la partie renfort du tour on peut activer cette carte, de plus on obtient la récompense associée à cette dernière quand on l'achète</t>
+  </si>
+  <si>
+    <t>vérifier si l'on peut aller sur l'ile 3,soleil</t>
+  </si>
+  <si>
+    <t>ajout à l'ile 3,soleil de l'exploit "La méduse" quand ce dernier est acheté, l'action décrite plus bas est effectuée et on obtient la récompense associée</t>
+  </si>
+  <si>
+    <t>ajout à l'ile 2,soleil de l'exploit "Le minotaure" quand ce dernier est acheté, l'action décrite plus bas est effectuée et on obtient la récompense associée</t>
+  </si>
+  <si>
+    <t>ajout à l'ile 3,soleil de l'exploit "Le miroir abyssal" quand ce dernier est acheté, l'action décrite plus bas est effectuée et on obtient la récompense associée</t>
+  </si>
+  <si>
+    <t>on va faire s'affronter toute les AI précédente pour voir laquelle est la plus performante sur des milliers(?) de matchs</t>
+  </si>
+  <si>
+    <t>vérifier si l'on peut aller sur l'ile 4,lune+soleil</t>
+  </si>
+  <si>
+    <t>ajout à l'ile 4,lune+soleil de l'exploit "La pince" quand ce dernier est acheté, l'action décrite plus bas est effectuée et on obtient la récompense associée</t>
+  </si>
+  <si>
+    <t>ajout à l'ile 4,lune+soleil de l'exploit "L'énigme" quand ce dernier est acheté, l'action décrite plus bas est effectuée et on obtient la récompense associée</t>
+  </si>
+  <si>
+    <t>ajout à l'ile 4,lune+soleil de l'exploit "l'Hydre" quand ce dernier est acheté, l'action décrite plus bas est effectuée et on obtient la récompense associée</t>
+  </si>
+  <si>
+    <t>toutes les AI précedemment créée vont s'affronter pour voir laquelle est la plus performante sur X parties (où X est supérieur à 1000?)</t>
+  </si>
+  <si>
+    <t>quand on a fini de forger/réaliser un exploit si l'on possède encore 2PdS et que l'on a pas déjà utiliser cette option on peut, en sacrifiant ces PdS refaire une action</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -775,7 +888,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -811,13 +924,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -852,15 +976,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Style de tableau 1" pivot="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
+    <tableStyle name="Style de tableau 1" pivot="0" count="0"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1169,28 +1296,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M85"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.1640625" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="24.1640625" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30" customWidth="1"/>
-    <col min="12" max="12" width="22.5" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1228,7 +1355,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1236,13 +1363,13 @@
         <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
@@ -1266,22 +1393,22 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F3" s="7">
         <v>1</v>
@@ -1299,28 +1426,28 @@
         <v>11</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
-        <f t="shared" ref="A4:A52" si="0">A3+1</f>
+        <f t="shared" ref="A4:A51" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F4" s="7">
         <v>1</v>
@@ -1342,22 +1469,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F5" s="7">
         <v>1</v>
@@ -1377,22 +1504,22 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
@@ -1412,7 +1539,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1421,13 +1548,13 @@
         <v>59</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
@@ -1442,10 +1569,10 @@
         <v>43385</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="206" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="206.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1454,10 +1581,12 @@
         <v>93</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="6" t="s">
+        <v>211</v>
+      </c>
       <c r="F8" s="7">
         <v>2</v>
       </c>
@@ -1466,7 +1595,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="127.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1475,10 +1604,12 @@
         <v>143</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>212</v>
+      </c>
       <c r="F9" s="7">
         <v>2</v>
       </c>
@@ -1487,7 +1618,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="2"/>
     </row>
-    <row r="10" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="159" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1499,7 +1630,9 @@
         <v>144</v>
       </c>
       <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6" t="s">
+        <v>213</v>
+      </c>
       <c r="F10" s="7">
         <v>2</v>
       </c>
@@ -1508,19 +1641,21 @@
       <c r="I10" s="6"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:13" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="48.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>146</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>214</v>
+      </c>
       <c r="F11" s="7">
         <v>2</v>
       </c>
@@ -1529,65 +1664,76 @@
       <c r="I11" s="6"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:13" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="206.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="7"/>
+      <c r="E12" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F12" s="7">
+        <v>3</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:13" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>148</v>
+        <v>71</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>150</v>
+        <v>70</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="7"/>
+      <c r="E13" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="F13" s="7">
+        <v>3</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:13" ht="189" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>84</v>
+        <v>147</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>86</v>
+        <v>148</v>
       </c>
       <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7"/>
+      <c r="E14" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="F14" s="7">
+        <v>3</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="2"/>
-      <c r="L14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:13" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1599,15 +1745,19 @@
         <v>73</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="7"/>
+      <c r="E15" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F15" s="7">
+        <v>3</v>
+      </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1616,17 +1766,21 @@
         <v>13</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
+      <c r="E16" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="F16" s="7">
+        <v>3</v>
+      </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
     </row>
-    <row r="17" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1635,17 +1789,19 @@
         <v>94</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="E17" s="6" t="s">
+        <v>220</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1657,14 +1813,16 @@
         <v>85</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="6" t="s">
+        <v>221</v>
+      </c>
       <c r="F18" s="7"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1676,207 +1834,226 @@
         <v>88</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="E19" s="6" t="s">
+        <v>222</v>
+      </c>
       <c r="F19" s="7"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
+    <row r="20" spans="1:10" ht="143.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
       <c r="B20" s="6" t="s">
-        <v>89</v>
+        <v>223</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>90</v>
+        <v>224</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="6" t="s">
+        <v>225</v>
+      </c>
       <c r="F20" s="7"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10" ht="155" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="174.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>A19+1</f>
+        <v>19</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="E21" s="6" t="s">
+        <v>226</v>
+      </c>
       <c r="F21" s="7"/>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="174.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
       <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="E22" s="6" t="s">
+        <v>227</v>
+      </c>
       <c r="F22" s="7"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="E23" s="6" t="s">
+        <v>228</v>
+      </c>
       <c r="F23" s="7"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
     </row>
-    <row r="24" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="E24" s="6" t="s">
+        <v>229</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
     </row>
-    <row r="25" spans="1:10" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>154</v>
+        <v>113</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+      <c r="E25" s="6" t="s">
+        <v>230</v>
+      </c>
       <c r="F25" s="7"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>115</v>
+        <v>152</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="E26" s="6" t="s">
+        <v>231</v>
+      </c>
       <c r="F26" s="7"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="64.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="E27" s="6" t="s">
+        <v>232</v>
+      </c>
       <c r="F27" s="7"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="E28" s="6" t="s">
+        <v>233</v>
+      </c>
       <c r="F28" s="7"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
-    <row r="29" spans="1:10" ht="138" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="159" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="E29" s="6" t="s">
+        <v>234</v>
+      </c>
       <c r="F29" s="7"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>102</v>
@@ -1885,17 +2062,19 @@
         <v>103</v>
       </c>
       <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="E30" s="6" t="s">
+        <v>235</v>
+      </c>
       <c r="F30" s="7"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:10" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>97</v>
@@ -1904,17 +2083,19 @@
         <v>104</v>
       </c>
       <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="E31" s="6" t="s">
+        <v>236</v>
+      </c>
       <c r="F31" s="7"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
     </row>
-    <row r="32" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>105</v>
@@ -1923,17 +2104,19 @@
         <v>106</v>
       </c>
       <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="E32" s="6" t="s">
+        <v>237</v>
+      </c>
       <c r="F32" s="7"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
     </row>
-    <row r="33" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="127.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>107</v>
@@ -1942,17 +2125,19 @@
         <v>108</v>
       </c>
       <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+      <c r="E33" s="18" t="s">
+        <v>239</v>
+      </c>
       <c r="F33" s="7"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:10" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>117</v>
@@ -1961,271 +2146,295 @@
         <v>118</v>
       </c>
       <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="E34" s="6" t="s">
+        <v>238</v>
+      </c>
       <c r="F34" s="7"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
     </row>
-    <row r="35" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>173</v>
+        <v>119</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>174</v>
+        <v>120</v>
       </c>
       <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="E35" s="6" t="s">
+        <v>240</v>
+      </c>
       <c r="F35" s="7"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
     </row>
-    <row r="36" spans="1:10" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="159" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+      <c r="E36" s="6" t="s">
+        <v>241</v>
+      </c>
       <c r="F36" s="7"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
     </row>
-    <row r="37" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
+      <c r="E37" s="6" t="s">
+        <v>244</v>
+      </c>
       <c r="F37" s="7"/>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
     </row>
-    <row r="38" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+      <c r="E38" s="6" t="s">
+        <v>242</v>
+      </c>
       <c r="F38" s="7"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
     </row>
-    <row r="39" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
+      <c r="E39" s="6" t="s">
+        <v>243</v>
+      </c>
       <c r="F39" s="7"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
     </row>
-    <row r="40" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+      <c r="E40" s="6" t="s">
+        <v>245</v>
+      </c>
       <c r="F40" s="7"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
     </row>
-    <row r="41" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="96" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>130</v>
+        <v>171</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>131</v>
+        <v>172</v>
       </c>
       <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
+      <c r="E41" s="6" t="s">
+        <v>246</v>
+      </c>
       <c r="F41" s="7"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
     </row>
-    <row r="42" spans="1:10" ht="87" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="80.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>175</v>
+        <v>132</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>176</v>
+        <v>133</v>
       </c>
       <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
+      <c r="E42" s="6" t="s">
+        <v>247</v>
+      </c>
       <c r="F42" s="7"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
     </row>
-    <row r="43" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+      <c r="E43" s="6" t="s">
+        <v>248</v>
+      </c>
       <c r="F43" s="7"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
     </row>
-    <row r="44" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
+      <c r="E44" s="6" t="s">
+        <v>250</v>
+      </c>
       <c r="F44" s="7"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
     </row>
-    <row r="45" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
+      <c r="E45" s="6" t="s">
+        <v>249</v>
+      </c>
       <c r="F45" s="7"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
     </row>
-    <row r="46" spans="1:10" ht="70" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
       <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
+      <c r="E46" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="F46" s="7"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
     </row>
-    <row r="47" spans="1:10" ht="104" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="111.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>140</v>
+        <v>190</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
+      <c r="E47" s="6" t="s">
+        <v>252</v>
+      </c>
       <c r="F47" s="7"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
     </row>
-    <row r="48" spans="1:10" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>195</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
       <c r="F48" s="7"/>
@@ -2234,10 +2443,10 @@
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
     </row>
-    <row r="49" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -2249,10 +2458,10 @@
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
     </row>
-    <row r="50" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
@@ -2264,10 +2473,10 @@
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
     </row>
-    <row r="51" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -2279,167 +2488,184 @@
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
     </row>
-    <row r="52" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
-        <f t="shared" si="0"/>
+    <row r="52" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="12"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L55" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="121.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J56" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="L56" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="6"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-    </row>
-    <row r="53" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="12"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C54" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C56" s="4" t="s">
+      <c r="M56" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D56" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I56" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J56" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L56" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="130" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J57" s="14" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="L57" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M57" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J58" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M58" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="M57" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="66" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="J58" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M58" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="34" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:13" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>56</v>
+      <c r="E59" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G59" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J59" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="I59" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J59" s="15" t="s">
-        <v>181</v>
-      </c>
       <c r="L59" s="2" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="M59" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="82" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>57</v>
+        <v>78</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>26</v>
@@ -2448,198 +2674,193 @@
         <v>160</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J60" s="14" t="s">
-        <v>161</v>
+        <v>22</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M60" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B61" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>78</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J61" s="14" t="s">
-        <v>22</v>
+        <v>178</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>22</v>
+        <v>170</v>
       </c>
       <c r="M61" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J62" s="14" t="s">
-        <v>182</v>
+        <v>69</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="M62" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B63" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>33</v>
+        <v>181</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>79</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G63" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I63" s="1"/>
+      <c r="L63" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="I63" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J63" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="L63" s="2" t="s">
-        <v>184</v>
-      </c>
       <c r="M63" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>29</v>
+        <v>165</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="I64" s="1"/>
       <c r="L64" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="M64" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="2:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>80</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>167</v>
+        <v>39</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I65" s="1"/>
       <c r="L65" s="2" t="s">
-        <v>163</v>
+        <v>54</v>
       </c>
       <c r="M65" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="66" spans="2:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B66" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>39</v>
+        <v>182</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I66" s="1"/>
       <c r="L66" s="2" t="s">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="M66" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="67" spans="2:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>184</v>
@@ -2647,150 +2868,123 @@
       <c r="D67" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E67" s="2" t="s">
-        <v>186</v>
+      <c r="E67" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I67" s="1"/>
       <c r="L67" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="M67" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="68" spans="2:13" ht="34" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>42</v>
+        <v>82</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="I68" s="1"/>
       <c r="L68" s="2" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="M68" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="69" spans="2:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:13" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B69" s="2" t="s">
-        <v>43</v>
+        <v>127</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E69" s="2" t="s">
-        <v>29</v>
+      <c r="E69" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I69" s="1"/>
       <c r="L69" s="2" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="M69" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="70" spans="2:13" ht="50" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B70" s="2" t="s">
-        <v>127</v>
+        <v>45</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>44</v>
+        <v>79</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I70" s="1"/>
       <c r="L70" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M70" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="71" spans="2:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>169</v>
-      </c>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I71" s="1"/>
       <c r="L71" s="2" t="s">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="M71" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="2:13" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="I72" s="1"/>
-      <c r="L72" s="2" t="s">
-        <v>170</v>
-      </c>
+    <row r="72" spans="2:13" ht="108" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M72" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="2:13" ht="108" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M73" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="74" spans="2:13" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="2:13" ht="75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="41.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="2:13" ht="75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#4 ajout du numéro de la release/milestone pour chaque slice
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -1299,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:A51"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,7 +1795,9 @@
       <c r="E17" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="F17" s="7"/>
+      <c r="F17" s="7">
+        <v>4</v>
+      </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
@@ -1816,7 +1818,9 @@
       <c r="E18" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="7">
+        <v>4</v>
+      </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
@@ -1837,7 +1841,9 @@
       <c r="E19" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="F19" s="7"/>
+      <c r="F19" s="7">
+        <v>4</v>
+      </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
@@ -1855,7 +1861,9 @@
       <c r="E20" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="7">
+        <v>4</v>
+      </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
@@ -1876,7 +1884,9 @@
       <c r="E21" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="7">
+        <v>4</v>
+      </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
       <c r="I21" s="6"/>
@@ -1897,7 +1907,9 @@
       <c r="E22" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F22" s="7"/>
+      <c r="F22" s="7">
+        <v>4</v>
+      </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
@@ -1918,7 +1930,9 @@
       <c r="E23" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="F23" s="7"/>
+      <c r="F23" s="7">
+        <v>5</v>
+      </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -1939,7 +1953,9 @@
       <c r="E24" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="F24" s="7"/>
+      <c r="F24" s="7">
+        <v>5</v>
+      </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -1960,7 +1976,9 @@
       <c r="E25" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="7">
+        <v>5</v>
+      </c>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
@@ -1981,7 +1999,9 @@
       <c r="E26" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="7">
+        <v>5</v>
+      </c>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -2002,7 +2022,9 @@
       <c r="E27" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="F27" s="7"/>
+      <c r="F27" s="7">
+        <v>6</v>
+      </c>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
@@ -2023,7 +2045,9 @@
       <c r="E28" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="F28" s="7"/>
+      <c r="F28" s="7">
+        <v>6</v>
+      </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -2044,7 +2068,9 @@
       <c r="E29" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="F29" s="7"/>
+      <c r="F29" s="7">
+        <v>6</v>
+      </c>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
@@ -2065,7 +2091,9 @@
       <c r="E30" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="F30" s="7"/>
+      <c r="F30" s="7">
+        <v>6</v>
+      </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
@@ -2086,7 +2114,9 @@
       <c r="E31" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="F31" s="7"/>
+      <c r="F31" s="7">
+        <v>6</v>
+      </c>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
@@ -2107,7 +2137,9 @@
       <c r="E32" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="F32" s="7"/>
+      <c r="F32" s="7">
+        <v>6</v>
+      </c>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
@@ -2128,7 +2160,9 @@
       <c r="E33" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="F33" s="7"/>
+      <c r="F33" s="7">
+        <v>6</v>
+      </c>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2149,7 +2183,9 @@
       <c r="E34" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="F34" s="7"/>
+      <c r="F34" s="7">
+        <v>6</v>
+      </c>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2170,7 +2206,9 @@
       <c r="E35" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="F35" s="7"/>
+      <c r="F35" s="7">
+        <v>7</v>
+      </c>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2191,7 +2229,9 @@
       <c r="E36" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="F36" s="7"/>
+      <c r="F36" s="7">
+        <v>7</v>
+      </c>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2212,7 +2252,9 @@
       <c r="E37" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="F37" s="7"/>
+      <c r="F37" s="7">
+        <v>7</v>
+      </c>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2233,7 +2275,9 @@
       <c r="E38" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="F38" s="7"/>
+      <c r="F38" s="7">
+        <v>7</v>
+      </c>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -2254,7 +2298,9 @@
       <c r="E39" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="F39" s="7"/>
+      <c r="F39" s="7">
+        <v>7</v>
+      </c>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2275,7 +2321,9 @@
       <c r="E40" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="F40" s="7"/>
+      <c r="F40" s="7">
+        <v>7</v>
+      </c>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
@@ -2296,7 +2344,9 @@
       <c r="E41" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="F41" s="7"/>
+      <c r="F41" s="7">
+        <v>7</v>
+      </c>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="6"/>
@@ -2317,7 +2367,9 @@
       <c r="E42" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="F42" s="7"/>
+      <c r="F42" s="7">
+        <v>8</v>
+      </c>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
       <c r="I42" s="6"/>
@@ -2338,7 +2390,9 @@
       <c r="E43" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="F43" s="7"/>
+      <c r="F43" s="7">
+        <v>8</v>
+      </c>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
@@ -2359,7 +2413,9 @@
       <c r="E44" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="F44" s="7"/>
+      <c r="F44" s="7">
+        <v>8</v>
+      </c>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
       <c r="I44" s="6"/>
@@ -2380,7 +2436,9 @@
       <c r="E45" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="F45" s="7"/>
+      <c r="F45" s="7">
+        <v>8</v>
+      </c>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
@@ -2401,7 +2459,9 @@
       <c r="E46" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="F46" s="7"/>
+      <c r="F46" s="7">
+        <v>8</v>
+      </c>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
@@ -2422,7 +2482,9 @@
       <c r="E47" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="F47" s="7"/>
+      <c r="F47" s="7">
+        <v>9</v>
+      </c>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>

</xml_diff>

<commit_message>
Correct honour cost. Feats add honour
Feats honour count add to the play honour also correct honour for Chest Feat
</commit_message>
<xml_diff>
--- a/suivi.xlsx
+++ b/suivi.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\PS5-18-19-DiceForge-EquipeG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bibi/Documents/PS5-18-19-DiceForge-EquipeG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D34C963C-57BA-4709-B6E9-5458B9843DA2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D31D509-5CC2-C042-AF7D-ADD48B17483D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28700" windowHeight="13060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
@@ -811,7 +811,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -979,9 +979,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Insatisfaisant" xfId="2" builtinId="27"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2">
@@ -1258,25 +1258,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" customWidth="1"/>
     <col min="10" max="10" width="30" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" customWidth="1"/>
+    <col min="12" max="12" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.5">
+    <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="78.75">
+    <row r="2" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="63">
+    <row r="3" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <f>A2+1</f>
         <v>2</v>
@@ -1391,7 +1391,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="63">
+    <row r="4" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A51" si="0">A3+1</f>
         <v>3</v>
@@ -1428,7 +1428,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="63">
+    <row r="5" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1463,7 +1463,7 @@
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
     </row>
-    <row r="6" spans="1:13" ht="78.75">
+    <row r="6" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1498,7 +1498,7 @@
       <c r="L6" s="14"/>
       <c r="M6" s="14"/>
     </row>
-    <row r="7" spans="1:13" ht="78.75">
+    <row r="7" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1531,7 +1531,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="204.75">
+    <row r="8" spans="1:13" ht="204" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1564,7 +1564,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="126">
+    <row r="9" spans="1:13" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1593,7 +1593,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="157.5">
+    <row r="10" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1616,7 +1616,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:13" ht="47.25">
+    <row r="11" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1639,7 +1639,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:13" ht="204.75">
+    <row r="12" spans="1:13" ht="187" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1662,7 +1662,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:13" ht="110.25">
+    <row r="13" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1685,7 +1685,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="6"/>
     </row>
-    <row r="14" spans="1:13" ht="110.25">
+    <row r="14" spans="1:13" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1708,7 +1708,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="1:13" ht="63">
+    <row r="15" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1732,7 +1732,7 @@
       <c r="J15" s="1"/>
       <c r="M15" s="14"/>
     </row>
-    <row r="16" spans="1:13" ht="78.75">
+    <row r="16" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1755,7 +1755,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" ht="141.75">
+    <row r="17" spans="1:10" ht="136" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1778,7 +1778,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" ht="94.5">
+    <row r="18" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1801,7 +1801,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="110.25">
+    <row r="19" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1824,7 +1824,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" ht="141.75">
+    <row r="20" spans="1:10" ht="136" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
         <v>77</v>
@@ -1844,7 +1844,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" ht="173.25">
+    <row r="21" spans="1:10" ht="170" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <f>A19+1</f>
         <v>19</v>
@@ -1867,7 +1867,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" ht="173.25">
+    <row r="22" spans="1:10" ht="153" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1890,7 +1890,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" ht="78.75">
+    <row r="23" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1913,7 +1913,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" ht="78.75">
+    <row r="24" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1936,7 +1936,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" ht="78.75">
+    <row r="25" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1959,7 +1959,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" ht="94.5">
+    <row r="26" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1982,7 +1982,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" ht="63">
+    <row r="27" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2005,7 +2005,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" ht="78.75">
+    <row r="28" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2028,7 +2028,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" ht="157.5">
+    <row r="29" spans="1:10" ht="153" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2051,7 +2051,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" ht="110.25">
+    <row r="30" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2074,7 +2074,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" ht="78.75">
+    <row r="31" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2097,7 +2097,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" ht="110.25">
+    <row r="32" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2120,7 +2120,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" ht="126">
+    <row r="33" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2143,7 +2143,7 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" ht="94.5">
+    <row r="34" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2166,7 +2166,7 @@
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" ht="78.75">
+    <row r="35" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2189,7 +2189,7 @@
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" ht="157.5">
+    <row r="36" spans="1:10" ht="153" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2212,7 +2212,7 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" ht="110.25">
+    <row r="37" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2235,7 +2235,7 @@
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" ht="78.75">
+    <row r="38" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2258,7 +2258,7 @@
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="1:10" ht="110.25">
+    <row r="39" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2281,7 +2281,7 @@
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="1:10" ht="110.25">
+    <row r="40" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2304,7 +2304,7 @@
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" ht="94.5">
+    <row r="41" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2327,7 +2327,7 @@
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="1:10" ht="78.75">
+    <row r="42" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2350,7 +2350,7 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" ht="110.25">
+    <row r="43" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2373,7 +2373,7 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="1:10" ht="110.25">
+    <row r="44" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2396,7 +2396,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10" ht="110.25">
+    <row r="45" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2419,7 +2419,7 @@
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10" ht="110.25">
+    <row r="46" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2442,7 +2442,7 @@
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="1:10" ht="110.25">
+    <row r="47" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2465,7 +2465,7 @@
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="1:10" ht="15.75">
+    <row r="48" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2480,7 +2480,7 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="49" spans="1:13" ht="15.75">
+    <row r="49" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2495,7 +2495,7 @@
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
-    <row r="50" spans="1:13" ht="15.75">
+    <row r="50" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2510,7 +2510,7 @@
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
-    <row r="51" spans="1:13" ht="15.75">
+    <row r="51" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2525,15 +2525,15 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="1:13" ht="15.75">
+    <row r="52" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B52" s="9"/>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C53" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B55" s="10" t="s">
         <v>162</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="120">
+    <row r="56" spans="1:13" ht="128" x14ac:dyDescent="0.2">
       <c r="B56" s="6" t="s">
         <v>170</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="60">
+    <row r="57" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="B57" s="6" t="s">
         <v>178</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>173</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="I57" s="6" t="s">
         <v>181</v>
@@ -2626,7 +2626,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="30">
+    <row r="58" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="B58" s="6" t="s">
         <v>185</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="75">
+    <row r="59" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="B59" s="6" t="s">
         <v>194</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B60" s="6" t="s">
         <v>200</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B61" s="6" t="s">
         <v>206</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="60">
+    <row r="62" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="B62" s="6" t="s">
         <v>212</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B63" s="6" t="s">
         <v>220</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B64" s="6" t="s">
         <v>225</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="65" spans="2:13">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B65" s="6" t="s">
         <v>228</v>
       </c>
@@ -2867,7 +2867,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="66" spans="2:13">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B66" s="6" t="s">
         <v>232</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="67" spans="2:13" ht="30">
+    <row r="67" spans="2:13" ht="32" x14ac:dyDescent="0.2">
       <c r="B67" s="6" t="s">
         <v>236</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="68" spans="2:13">
+    <row r="68" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B68" s="6" t="s">
         <v>239</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="69" spans="2:13" ht="60">
+    <row r="69" spans="2:13" ht="48" x14ac:dyDescent="0.2">
       <c r="B69" s="6" t="s">
         <v>243</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="70" spans="2:13">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B70" s="6" t="s">
         <v>249</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="71" spans="2:13">
+    <row r="71" spans="2:13" x14ac:dyDescent="0.2">
       <c r="I71" s="14"/>
       <c r="L71" s="6" t="s">
         <v>253</v>
@@ -3011,15 +3011,15 @@
         <v>231</v>
       </c>
     </row>
-    <row r="72" spans="2:13" ht="108" customHeight="1">
+    <row r="72" spans="2:13" ht="108" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M72" s="6" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="74" spans="2:13" ht="75" customHeight="1"/>
-    <row r="82" ht="41.25" customHeight="1"/>
-    <row r="83" ht="19.5" customHeight="1"/>
-    <row r="84" ht="45" customHeight="1"/>
+    <row r="74" spans="2:13" ht="75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="41.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="45" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>